<commit_message>
v0.1 - something works but some issues
</commit_message>
<xml_diff>
--- a/database/steel_data.xlsx
+++ b/database/steel_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PLANiT\github\macc_steel\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8435790-B742-4534-8B41-B881E75A1141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EDBF0F-0459-4B7D-8F07-1482A5425DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27920" yWindow="720" windowWidth="26350" windowHeight="14720" tabRatio="620" activeTab="1" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
   </bookViews>
@@ -211,10 +211,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>remained_lifespan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>material</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -232,6 +228,10 @@
   </si>
   <si>
     <t>introduction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>introduced_year</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -728,7 +728,7 @@
         <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -760,10 +760,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -840,10 +840,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -905,14 +905,14 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1">
         <v>2025</v>
@@ -1164,82 +1164,82 @@
         <v>7</v>
       </c>
       <c r="B4" s="5">
-        <v>1.6561115100472845</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>6.8203698630888576</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5">
-        <v>1.4137603139272703</v>
+        <v>0</v>
       </c>
       <c r="E4" s="5">
-        <v>4.3586868316947838</v>
+        <v>0</v>
       </c>
       <c r="F4" s="5">
-        <v>9.5169563479933696</v>
+        <v>0</v>
       </c>
       <c r="G4" s="5">
-        <v>6.6592244131241145</v>
+        <v>0</v>
       </c>
       <c r="H4" s="5">
-        <v>3.2346583782178726</v>
+        <v>0</v>
       </c>
       <c r="I4" s="5">
-        <v>8.4298844355731966</v>
+        <v>0</v>
       </c>
       <c r="J4" s="5">
-        <v>2.0837137856376531E-2</v>
+        <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>7.801618608794608</v>
+        <v>0</v>
       </c>
       <c r="L4" s="5">
-        <v>1.1747432563255356</v>
+        <v>0</v>
       </c>
       <c r="M4" s="5">
-        <v>9.2189855539967063</v>
+        <v>0</v>
       </c>
       <c r="N4" s="5">
-        <v>5.6389770014244593</v>
+        <v>0</v>
       </c>
       <c r="O4" s="5">
-        <v>9.3557448426025598</v>
+        <v>0</v>
       </c>
       <c r="P4" s="5">
-        <v>2.5307863577058676</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="5">
-        <v>1.8798425218320436</v>
+        <v>0</v>
       </c>
       <c r="R4" s="5">
-        <v>4.9777650025283062</v>
+        <v>0</v>
       </c>
       <c r="S4" s="5">
-        <v>2.470635282434567</v>
+        <v>0</v>
       </c>
       <c r="T4" s="5">
-        <v>8.3448632095880253</v>
+        <v>0</v>
       </c>
       <c r="U4" s="5">
-        <v>2.8797087757874475</v>
+        <v>0</v>
       </c>
       <c r="V4" s="5">
-        <v>4.8495072111122131</v>
+        <v>0</v>
       </c>
       <c r="W4" s="5">
-        <v>0.6494650243068445</v>
+        <v>0</v>
       </c>
       <c r="X4" s="5">
-        <v>4.0400013877281555</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="5">
-        <v>8.7109696253244202</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="5">
-        <v>2.5086878384546196</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="5">
-        <v>1.6351143304444082</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.4">
@@ -1426,7 +1426,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1">
         <v>2025</v>
@@ -1940,7 +1940,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1">
         <v>2025</v>
@@ -2463,19 +2463,19 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -2495,7 +2495,7 @@
         <v>4000</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -2515,7 +2515,7 @@
         <v>3000</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -2535,7 +2535,7 @@
         <v>1500</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -2555,7 +2555,7 @@
         <v>1500</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -2568,13 +2568,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E234AF8D-964B-419F-969D-C9FD34B2C8AE}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1">
         <v>2025</v>
@@ -2785,40 +2787,40 @@
         <v>40</v>
       </c>
       <c r="P3" s="4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R3" s="4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="S3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="U3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="V3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="W3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="X3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -2868,40 +2870,40 @@
         <v>67</v>
       </c>
       <c r="P4">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="Q4">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="R4">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="S4">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="T4">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="U4">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="V4">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="W4">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="X4">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="Y4">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="Z4">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="AA4">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2920,7 +2922,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1">
         <v>2025</v>
@@ -3172,51 +3174,51 @@
       </c>
       <c r="P3" s="3">
         <f>capex!P3*0.05</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="3">
         <f>capex!Q3*0.05</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="R3" s="3">
         <f>capex!R3*0.05</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="S3" s="3">
         <f>capex!S3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="3">
         <f>capex!T3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" s="3">
         <f>capex!U3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="3">
         <f>capex!V3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" s="3">
         <f>capex!W3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" s="3">
         <f>capex!X3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="3">
         <f>capex!Y3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="3">
         <f>capex!Z3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="3">
         <f>capex!AA3*0.05</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -3281,51 +3283,51 @@
       </c>
       <c r="P4" s="3">
         <f>capex!P4*0.05</f>
-        <v>3.3000000000000003</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="3">
         <f>capex!Q4*0.05</f>
-        <v>3.25</v>
+        <v>1</v>
       </c>
       <c r="R4" s="3">
         <f>capex!R4*0.05</f>
-        <v>3.2</v>
+        <v>1</v>
       </c>
       <c r="S4" s="3">
         <f>capex!S4*0.05</f>
-        <v>3.1500000000000004</v>
+        <v>1</v>
       </c>
       <c r="T4" s="3">
         <f>capex!T4*0.05</f>
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="U4" s="3">
         <f>capex!U4*0.05</f>
-        <v>3.0500000000000003</v>
+        <v>1</v>
       </c>
       <c r="V4" s="3">
         <f>capex!V4*0.05</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W4" s="3">
         <f>capex!W4*0.05</f>
-        <v>2.95</v>
+        <v>1</v>
       </c>
       <c r="X4" s="3">
         <f>capex!X4*0.05</f>
-        <v>2.9000000000000004</v>
+        <v>1</v>
       </c>
       <c r="Y4" s="3">
         <f>capex!Y4*0.05</f>
-        <v>2.85</v>
+        <v>1</v>
       </c>
       <c r="Z4" s="3">
         <f>capex!Z4*0.05</f>
-        <v>2.8000000000000003</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="3">
         <f>capex!AA4*0.05</f>
-        <v>2.75</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3344,7 +3346,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1">
         <v>2025</v>
@@ -3596,51 +3598,51 @@
       </c>
       <c r="P3" s="3">
         <f>capex!P3*0.25</f>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="3">
         <f>capex!Q3*0.25</f>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="R3" s="3">
         <f>capex!R3*0.25</f>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="S3" s="3">
         <f>capex!S3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T3" s="3">
         <f>capex!T3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U3" s="3">
         <f>capex!U3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V3" s="3">
         <f>capex!V3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W3" s="3">
         <f>capex!W3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X3" s="3">
         <f>capex!X3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="3">
         <f>capex!Y3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="3">
         <f>capex!Z3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="3">
         <f>capex!AA3*0.25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -3705,51 +3707,51 @@
       </c>
       <c r="P4" s="3">
         <f>capex!P4*0.25</f>
-        <v>16.5</v>
+        <v>5</v>
       </c>
       <c r="Q4" s="3">
         <f>capex!Q4*0.25</f>
-        <v>16.25</v>
+        <v>5</v>
       </c>
       <c r="R4" s="3">
         <f>capex!R4*0.25</f>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="S4" s="3">
         <f>capex!S4*0.25</f>
-        <v>15.75</v>
+        <v>5</v>
       </c>
       <c r="T4" s="3">
         <f>capex!T4*0.25</f>
-        <v>15.5</v>
+        <v>5</v>
       </c>
       <c r="U4" s="3">
         <f>capex!U4*0.25</f>
-        <v>15.25</v>
+        <v>5</v>
       </c>
       <c r="V4" s="3">
         <f>capex!V4*0.25</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="W4" s="3">
         <f>capex!W4*0.25</f>
-        <v>14.75</v>
+        <v>5</v>
       </c>
       <c r="X4" s="3">
         <f>capex!X4*0.25</f>
-        <v>14.5</v>
+        <v>5</v>
       </c>
       <c r="Y4" s="3">
         <f>capex!Y4*0.25</f>
-        <v>14.25</v>
+        <v>5</v>
       </c>
       <c r="Z4" s="3">
         <f>capex!Z4*0.25</f>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AA4" s="3">
         <f>capex!AA4*0.25</f>
-        <v>13.75</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3763,7 +3765,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3775,13 +3777,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -3836,7 +3838,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1">
         <v>2025</v>
@@ -4268,7 +4270,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1">
         <v>2025</v>
@@ -4697,7 +4699,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1">
         <v>2025</v>

</xml_diff>

<commit_message>
v0.1 - System-level emission (working version. simple) v0.2 - System-wide emission (take longer time, and still being tested)
</commit_message>
<xml_diff>
--- a/database/steel_data.xlsx
+++ b/database/steel_data.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PLANiT\github\macc_steel\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064475A1-D367-4864-81FC-9F5674CC779D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED14111-91C8-40B0-AEBD-460223846C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="1632" windowWidth="37776" windowHeight="14724" tabRatio="620" activeTab="5" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
+    <workbookView xWindow="192" yWindow="348" windowWidth="37152" windowHeight="14724" tabRatio="620" activeTab="2" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="18" r:id="rId1"/>
     <sheet name="baseline" sheetId="7" r:id="rId2"/>
-    <sheet name="capex" sheetId="13" r:id="rId3"/>
-    <sheet name="opex" sheetId="14" r:id="rId4"/>
-    <sheet name="renewal" sheetId="15" r:id="rId5"/>
-    <sheet name="technology" sheetId="19" r:id="rId6"/>
-    <sheet name="technology_ei" sheetId="21" r:id="rId7"/>
-    <sheet name="emission" sheetId="23" r:id="rId8"/>
-    <sheet name="material_cost" sheetId="11" r:id="rId9"/>
-    <sheet name="material_emission" sheetId="12" r:id="rId10"/>
-    <sheet name="material_efficiency" sheetId="17" r:id="rId11"/>
-    <sheet name="technology_fuel_pairs" sheetId="5" r:id="rId12"/>
-    <sheet name="technology_material_pairs" sheetId="6" r:id="rId13"/>
-    <sheet name="fuel_cost" sheetId="8" r:id="rId14"/>
-    <sheet name="fuel_efficiency" sheetId="16" r:id="rId15"/>
-    <sheet name="fuel_emission" sheetId="10" r:id="rId16"/>
+    <sheet name="emission_system" sheetId="24" r:id="rId3"/>
+    <sheet name="capex" sheetId="13" r:id="rId4"/>
+    <sheet name="opex" sheetId="14" r:id="rId5"/>
+    <sheet name="renewal" sheetId="15" r:id="rId6"/>
+    <sheet name="technology" sheetId="19" r:id="rId7"/>
+    <sheet name="technology_ei" sheetId="21" r:id="rId8"/>
+    <sheet name="emission" sheetId="23" r:id="rId9"/>
+    <sheet name="material_cost" sheetId="11" r:id="rId10"/>
+    <sheet name="material_emission" sheetId="12" r:id="rId11"/>
+    <sheet name="material_efficiency" sheetId="17" r:id="rId12"/>
+    <sheet name="technology_fuel_pairs" sheetId="5" r:id="rId13"/>
+    <sheet name="technology_material_pairs" sheetId="6" r:id="rId14"/>
+    <sheet name="fuel_cost" sheetId="8" r:id="rId15"/>
+    <sheet name="fuel_efficiency" sheetId="16" r:id="rId16"/>
+    <sheet name="fuel_emission" sheetId="10" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>BF-BOF</t>
   </si>
@@ -249,11 +250,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>scope1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>scope2</t>
+    <t>tonCO2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -665,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21BDFBF-8BC3-41DF-97CA-33C5F9721F61}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -761,6 +758,14 @@
         <v>42</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -768,10 +773,12 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E18AD-1C92-4B5C-962D-792F4AC09175}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9059A3E3-467F-433B-AAF0-DA415330A29D}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection sqref="A1:AA1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1200,6 +1207,440 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E18AD-1C92-4B5C-962D-792F4AC09175}">
+  <dimension ref="A1:AA5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AA5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="27" width="9.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1">
+        <v>2025</v>
+      </c>
+      <c r="C1">
+        <v>2026</v>
+      </c>
+      <c r="D1">
+        <v>2027</v>
+      </c>
+      <c r="E1">
+        <v>2028</v>
+      </c>
+      <c r="F1">
+        <v>2029</v>
+      </c>
+      <c r="G1">
+        <v>2030</v>
+      </c>
+      <c r="H1">
+        <v>2031</v>
+      </c>
+      <c r="I1">
+        <v>2032</v>
+      </c>
+      <c r="J1">
+        <v>2033</v>
+      </c>
+      <c r="K1">
+        <v>2034</v>
+      </c>
+      <c r="L1">
+        <v>2035</v>
+      </c>
+      <c r="M1">
+        <v>2036</v>
+      </c>
+      <c r="N1">
+        <v>2037</v>
+      </c>
+      <c r="O1">
+        <v>2038</v>
+      </c>
+      <c r="P1">
+        <v>2039</v>
+      </c>
+      <c r="Q1">
+        <v>2040</v>
+      </c>
+      <c r="R1">
+        <v>2041</v>
+      </c>
+      <c r="S1">
+        <v>2042</v>
+      </c>
+      <c r="T1">
+        <v>2043</v>
+      </c>
+      <c r="U1">
+        <v>2044</v>
+      </c>
+      <c r="V1">
+        <v>2045</v>
+      </c>
+      <c r="W1">
+        <v>2046</v>
+      </c>
+      <c r="X1">
+        <v>2047</v>
+      </c>
+      <c r="Y1">
+        <v>2048</v>
+      </c>
+      <c r="Z1">
+        <v>2049</v>
+      </c>
+      <c r="AA1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5">
+        <v>10</v>
+      </c>
+      <c r="J2" s="5">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5">
+        <v>10</v>
+      </c>
+      <c r="L2" s="5">
+        <v>10</v>
+      </c>
+      <c r="M2" s="5">
+        <v>10</v>
+      </c>
+      <c r="N2" s="5">
+        <v>10</v>
+      </c>
+      <c r="O2" s="5">
+        <v>10</v>
+      </c>
+      <c r="P2" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>10</v>
+      </c>
+      <c r="R2" s="5">
+        <v>10</v>
+      </c>
+      <c r="S2" s="5">
+        <v>10</v>
+      </c>
+      <c r="T2" s="5">
+        <v>10</v>
+      </c>
+      <c r="U2" s="5">
+        <v>10</v>
+      </c>
+      <c r="V2" s="5">
+        <v>10</v>
+      </c>
+      <c r="W2" s="5">
+        <v>10</v>
+      </c>
+      <c r="X2" s="5">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>10</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0</v>
+      </c>
+      <c r="X3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0</v>
+      </c>
+      <c r="X4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="5">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5">
+        <v>3</v>
+      </c>
+      <c r="K5" s="5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="5">
+        <v>3</v>
+      </c>
+      <c r="N5" s="5">
+        <v>3</v>
+      </c>
+      <c r="O5" s="5">
+        <v>3</v>
+      </c>
+      <c r="P5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>3</v>
+      </c>
+      <c r="R5" s="5">
+        <v>3</v>
+      </c>
+      <c r="S5" s="5">
+        <v>3</v>
+      </c>
+      <c r="T5" s="5">
+        <v>3</v>
+      </c>
+      <c r="U5" s="5">
+        <v>3</v>
+      </c>
+      <c r="V5" s="5">
+        <v>3</v>
+      </c>
+      <c r="W5" s="5">
+        <v>3</v>
+      </c>
+      <c r="X5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CF035B-C14B-46B7-A841-579E94220A37}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -1628,7 +2069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A5865B-B011-402F-A09D-739FDD6B0E90}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -1727,7 +2168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A8B42D-00EB-470C-A0D2-7C21A6CB877B}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1815,7 +2256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251D8908-2320-4E41-AC8F-86BD7BF58C9B}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
@@ -2329,7 +2770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC1A385-697C-4C01-B126-79A22BD0CC72}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
@@ -2843,12 +3284,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EB8FDB-F47B-40C2-8266-6700BCAB2D8C}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2941,82 +3382,82 @@
         <v>5</v>
       </c>
       <c r="B2" s="5">
-        <v>6.2600453911352592</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5">
-        <v>8.8222245042937839</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5">
-        <v>4.8668853685625946</v>
+        <v>15</v>
       </c>
       <c r="E2" s="5">
-        <v>3.0027339992948447</v>
+        <v>15</v>
       </c>
       <c r="F2" s="5">
-        <v>12.316434020161935</v>
+        <v>15</v>
       </c>
       <c r="G2" s="5">
-        <v>9.1604563428165449</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5">
-        <v>13.810504059621291</v>
+        <v>15</v>
       </c>
       <c r="I2" s="5">
-        <v>13.678304827571088</v>
+        <v>15</v>
       </c>
       <c r="J2" s="5">
-        <v>5.8399342077426173</v>
+        <v>15</v>
       </c>
       <c r="K2" s="5">
-        <v>2.560914432207829</v>
+        <v>15</v>
       </c>
       <c r="L2" s="5">
-        <v>5.0246792755547727</v>
+        <v>15</v>
       </c>
       <c r="M2" s="5">
-        <v>7.5294774046140711</v>
+        <v>15</v>
       </c>
       <c r="N2" s="5">
-        <v>1.9541670348732643</v>
+        <v>15</v>
       </c>
       <c r="O2" s="5">
-        <v>13.207174085612678</v>
+        <v>15</v>
       </c>
       <c r="P2" s="5">
-        <v>2.1123798485142267</v>
+        <v>15</v>
       </c>
       <c r="Q2" s="5">
-        <v>8.2771658498784042</v>
+        <v>15</v>
       </c>
       <c r="R2" s="5">
-        <v>11.435579213869961</v>
+        <v>15</v>
       </c>
       <c r="S2" s="5">
-        <v>3.9924456653586322</v>
+        <v>15</v>
       </c>
       <c r="T2" s="5">
-        <v>2.2337207330716131</v>
+        <v>15</v>
       </c>
       <c r="U2" s="5">
-        <v>0.77075067579372769</v>
+        <v>15</v>
       </c>
       <c r="V2" s="5">
-        <v>7.4480948670040483</v>
+        <v>15</v>
       </c>
       <c r="W2" s="5">
-        <v>9.2154154285436807</v>
+        <v>15</v>
       </c>
       <c r="X2" s="5">
-        <v>9.2716405592341573</v>
+        <v>15</v>
       </c>
       <c r="Y2" s="5">
-        <v>12.967771240834429</v>
+        <v>15</v>
       </c>
       <c r="Z2" s="5">
-        <v>0.57482413439813695</v>
+        <v>15</v>
       </c>
       <c r="AA2" s="5">
-        <v>4.9093381539763445</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
@@ -3024,82 +3465,82 @@
         <v>6</v>
       </c>
       <c r="B3" s="5">
-        <v>6.0928105811331736</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5">
-        <v>10.920004594456977</v>
+        <v>7</v>
       </c>
       <c r="D3" s="5">
-        <v>10.31641722809619</v>
+        <v>7</v>
       </c>
       <c r="E3" s="5">
-        <v>11.231570014907881</v>
+        <v>7</v>
       </c>
       <c r="F3" s="5">
-        <v>4.0300577869180412</v>
+        <v>7</v>
       </c>
       <c r="G3" s="5">
-        <v>9.7931874255999407</v>
+        <v>7</v>
       </c>
       <c r="H3" s="5">
-        <v>6.5855699920290354</v>
+        <v>7</v>
       </c>
       <c r="I3" s="5">
-        <v>12.645957910868292</v>
+        <v>7</v>
       </c>
       <c r="J3" s="5">
-        <v>9.0111096831596385</v>
+        <v>7</v>
       </c>
       <c r="K3" s="5">
-        <v>14.461253731910586</v>
+        <v>7</v>
       </c>
       <c r="L3" s="5">
-        <v>8.9799456481388624</v>
+        <v>7</v>
       </c>
       <c r="M3" s="5">
-        <v>4.7150586178587268</v>
+        <v>7</v>
       </c>
       <c r="N3" s="5">
-        <v>5.4839121890832141</v>
+        <v>7</v>
       </c>
       <c r="O3" s="5">
-        <v>10.122550689063209</v>
+        <v>7</v>
       </c>
       <c r="P3" s="5">
-        <v>7.8280462780875242</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="5">
-        <v>7.6429173482145618</v>
+        <v>7</v>
       </c>
       <c r="R3" s="5">
-        <v>7.3949426293514016</v>
+        <v>7</v>
       </c>
       <c r="S3" s="5">
-        <v>5.9836552397334621</v>
+        <v>7</v>
       </c>
       <c r="T3" s="5">
-        <v>14.767485384903011</v>
+        <v>7</v>
       </c>
       <c r="U3" s="5">
-        <v>14.941741866675336</v>
+        <v>7</v>
       </c>
       <c r="V3" s="5">
-        <v>7.7439303214902528</v>
+        <v>7</v>
       </c>
       <c r="W3" s="5">
-        <v>2.2664469848803375</v>
+        <v>7</v>
       </c>
       <c r="X3" s="5">
-        <v>13.544815043150813</v>
+        <v>7</v>
       </c>
       <c r="Y3" s="5">
-        <v>6.4222308368027994</v>
+        <v>7</v>
       </c>
       <c r="Z3" s="5">
-        <v>13.586164555760988</v>
+        <v>7</v>
       </c>
       <c r="AA3" s="5">
-        <v>4.7729454920000585</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -3107,52 +3548,52 @@
         <v>7</v>
       </c>
       <c r="B4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="5">
         <v>0</v>
@@ -3190,82 +3631,82 @@
         <v>8</v>
       </c>
       <c r="B5" s="5">
-        <v>1.5656079326091326</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5">
-        <v>7.0696725603625747</v>
+        <v>3</v>
       </c>
       <c r="D5" s="5">
-        <v>13.930561403523109</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5">
-        <v>1.8108541081271028</v>
+        <v>3</v>
       </c>
       <c r="F5" s="5">
-        <v>9.8977810969127145</v>
+        <v>3</v>
       </c>
       <c r="G5" s="5">
-        <v>8.9157542243891523</v>
+        <v>3</v>
       </c>
       <c r="H5" s="5">
-        <v>1.4197410500231373</v>
+        <v>3</v>
       </c>
       <c r="I5" s="5">
-        <v>14.42293937901222</v>
+        <v>3</v>
       </c>
       <c r="J5" s="5">
-        <v>5.7060995832871946</v>
+        <v>3</v>
       </c>
       <c r="K5" s="5">
-        <v>8.1914860415473392</v>
+        <v>3</v>
       </c>
       <c r="L5" s="5">
-        <v>1.1389909220565793</v>
+        <v>3</v>
       </c>
       <c r="M5" s="5">
-        <v>12.153650602918825</v>
+        <v>3</v>
       </c>
       <c r="N5" s="5">
-        <v>1.510531126422946</v>
+        <v>3</v>
       </c>
       <c r="O5" s="5">
-        <v>13.090121511788489</v>
+        <v>3</v>
       </c>
       <c r="P5" s="5">
-        <v>0.54059712332527765</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="5">
-        <v>3.7045329437070307</v>
+        <v>3</v>
       </c>
       <c r="R5" s="5">
-        <v>3.0330638243461121</v>
+        <v>3</v>
       </c>
       <c r="S5" s="5">
-        <v>12.903065697567044</v>
+        <v>3</v>
       </c>
       <c r="T5" s="5">
-        <v>1.4698172604967619</v>
+        <v>3</v>
       </c>
       <c r="U5" s="5">
-        <v>13.294158844375065</v>
+        <v>3</v>
       </c>
       <c r="V5" s="5">
-        <v>1.9401206045700869</v>
+        <v>3</v>
       </c>
       <c r="W5" s="5">
-        <v>11.556833436996552</v>
+        <v>3</v>
       </c>
       <c r="X5" s="5">
-        <v>10.776514785179515</v>
+        <v>3</v>
       </c>
       <c r="Y5" s="5">
-        <v>4.5405047745340825</v>
+        <v>3</v>
       </c>
       <c r="Z5" s="5">
-        <v>10.189852738682372</v>
+        <v>3</v>
       </c>
       <c r="AA5" s="5">
-        <v>0.64474612191384173</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.4">
@@ -3273,82 +3714,82 @@
         <v>9</v>
       </c>
       <c r="B6" s="5">
-        <v>5.6458240477817503</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5">
-        <v>12.11004514404361</v>
+        <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>2.4811179390953697</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5">
-        <v>6.1671767253971428</v>
+        <v>10</v>
       </c>
       <c r="F6" s="5">
-        <v>7.5454106189369359</v>
+        <v>10</v>
       </c>
       <c r="G6" s="5">
-        <v>7.0635669710864448</v>
+        <v>10</v>
       </c>
       <c r="H6" s="5">
-        <v>0.18246921511723524</v>
+        <v>10</v>
       </c>
       <c r="I6" s="5">
-        <v>3.4895307493457715</v>
+        <v>10</v>
       </c>
       <c r="J6" s="5">
-        <v>11.59767902500657</v>
+        <v>10</v>
       </c>
       <c r="K6" s="5">
-        <v>7.0683511784111568</v>
+        <v>10</v>
       </c>
       <c r="L6" s="5">
-        <v>0.64911250216048266</v>
+        <v>10</v>
       </c>
       <c r="M6" s="5">
-        <v>0.44520733666444823</v>
+        <v>10</v>
       </c>
       <c r="N6" s="5">
-        <v>8.9341169520372112</v>
+        <v>10</v>
       </c>
       <c r="O6" s="5">
-        <v>0.62570928049550445</v>
+        <v>10</v>
       </c>
       <c r="P6" s="5">
-        <v>8.9725944611639665</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="5">
-        <v>9.5227323982664096</v>
+        <v>10</v>
       </c>
       <c r="R6" s="5">
-        <v>12.414087553790218</v>
+        <v>10</v>
       </c>
       <c r="S6" s="5">
-        <v>1.7434432341620525</v>
+        <v>10</v>
       </c>
       <c r="T6" s="5">
-        <v>14.364541169192789</v>
+        <v>10</v>
       </c>
       <c r="U6" s="5">
-        <v>11.089944690516745</v>
+        <v>10</v>
       </c>
       <c r="V6" s="5">
-        <v>11.092578252638637</v>
+        <v>10</v>
       </c>
       <c r="W6" s="5">
-        <v>14.787616392537849</v>
+        <v>10</v>
       </c>
       <c r="X6" s="5">
-        <v>6.8072585730220982</v>
+        <v>10</v>
       </c>
       <c r="Y6" s="5">
-        <v>10.053584208006448</v>
+        <v>10</v>
       </c>
       <c r="Z6" s="5">
-        <v>6.4915980484470079</v>
+        <v>10</v>
       </c>
       <c r="AA6" s="5">
-        <v>9.8008766827123228</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3362,7 +3803,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3480,6 +3921,437 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E683ACB1-236C-41D9-AD28-376C61929EF9}">
+  <dimension ref="A1:AA5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:AA2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>2025</v>
+      </c>
+      <c r="C1">
+        <v>2026</v>
+      </c>
+      <c r="D1">
+        <v>2027</v>
+      </c>
+      <c r="E1">
+        <v>2028</v>
+      </c>
+      <c r="F1">
+        <v>2029</v>
+      </c>
+      <c r="G1">
+        <v>2030</v>
+      </c>
+      <c r="H1">
+        <v>2031</v>
+      </c>
+      <c r="I1">
+        <v>2032</v>
+      </c>
+      <c r="J1">
+        <v>2033</v>
+      </c>
+      <c r="K1">
+        <v>2034</v>
+      </c>
+      <c r="L1">
+        <v>2035</v>
+      </c>
+      <c r="M1">
+        <v>2036</v>
+      </c>
+      <c r="N1">
+        <v>2037</v>
+      </c>
+      <c r="O1">
+        <v>2038</v>
+      </c>
+      <c r="P1">
+        <v>2039</v>
+      </c>
+      <c r="Q1">
+        <v>2040</v>
+      </c>
+      <c r="R1">
+        <v>2041</v>
+      </c>
+      <c r="S1">
+        <v>2042</v>
+      </c>
+      <c r="T1">
+        <v>2043</v>
+      </c>
+      <c r="U1">
+        <v>2044</v>
+      </c>
+      <c r="V1">
+        <v>2045</v>
+      </c>
+      <c r="W1">
+        <v>2046</v>
+      </c>
+      <c r="X1">
+        <v>2047</v>
+      </c>
+      <c r="Y1">
+        <v>2048</v>
+      </c>
+      <c r="Z1">
+        <v>2049</v>
+      </c>
+      <c r="AA1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>500000</v>
+      </c>
+      <c r="C2">
+        <v>200000</v>
+      </c>
+      <c r="D2">
+        <v>200000</v>
+      </c>
+      <c r="E2">
+        <v>200000</v>
+      </c>
+      <c r="F2">
+        <v>200000</v>
+      </c>
+      <c r="G2">
+        <v>200000</v>
+      </c>
+      <c r="H2">
+        <v>200000</v>
+      </c>
+      <c r="I2">
+        <v>200000</v>
+      </c>
+      <c r="J2">
+        <v>200000</v>
+      </c>
+      <c r="K2">
+        <v>200000</v>
+      </c>
+      <c r="L2">
+        <v>100000</v>
+      </c>
+      <c r="M2">
+        <v>100000</v>
+      </c>
+      <c r="N2">
+        <v>100000</v>
+      </c>
+      <c r="O2">
+        <v>100000</v>
+      </c>
+      <c r="P2">
+        <v>100000</v>
+      </c>
+      <c r="Q2">
+        <v>50000</v>
+      </c>
+      <c r="R2">
+        <v>50000</v>
+      </c>
+      <c r="S2">
+        <v>50000</v>
+      </c>
+      <c r="T2">
+        <v>50000</v>
+      </c>
+      <c r="U2">
+        <v>50000</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>500000</v>
+      </c>
+      <c r="C3">
+        <v>500000</v>
+      </c>
+      <c r="D3">
+        <v>500000</v>
+      </c>
+      <c r="E3">
+        <v>500000</v>
+      </c>
+      <c r="F3">
+        <v>500000</v>
+      </c>
+      <c r="G3">
+        <v>500000</v>
+      </c>
+      <c r="H3">
+        <v>500000</v>
+      </c>
+      <c r="I3">
+        <v>500000</v>
+      </c>
+      <c r="J3">
+        <v>500000</v>
+      </c>
+      <c r="K3">
+        <v>200000</v>
+      </c>
+      <c r="L3">
+        <v>200000</v>
+      </c>
+      <c r="M3">
+        <v>200000</v>
+      </c>
+      <c r="N3">
+        <v>200000</v>
+      </c>
+      <c r="O3">
+        <v>200000</v>
+      </c>
+      <c r="P3">
+        <v>200000</v>
+      </c>
+      <c r="Q3">
+        <v>200000</v>
+      </c>
+      <c r="R3">
+        <v>200000</v>
+      </c>
+      <c r="S3">
+        <v>200000</v>
+      </c>
+      <c r="T3">
+        <v>200000</v>
+      </c>
+      <c r="U3">
+        <v>200000</v>
+      </c>
+      <c r="V3">
+        <v>200000</v>
+      </c>
+      <c r="W3">
+        <v>200000</v>
+      </c>
+      <c r="X3">
+        <v>200000</v>
+      </c>
+      <c r="Y3">
+        <v>200000</v>
+      </c>
+      <c r="Z3">
+        <v>200000</v>
+      </c>
+      <c r="AA3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>100000</v>
+      </c>
+      <c r="C4">
+        <v>100000</v>
+      </c>
+      <c r="D4">
+        <v>100000</v>
+      </c>
+      <c r="E4">
+        <v>100000</v>
+      </c>
+      <c r="F4">
+        <v>100000</v>
+      </c>
+      <c r="G4">
+        <v>100000</v>
+      </c>
+      <c r="H4">
+        <v>100000</v>
+      </c>
+      <c r="I4">
+        <v>100000</v>
+      </c>
+      <c r="J4">
+        <v>100000</v>
+      </c>
+      <c r="K4">
+        <v>100000</v>
+      </c>
+      <c r="L4">
+        <v>100000</v>
+      </c>
+      <c r="M4">
+        <v>100000</v>
+      </c>
+      <c r="N4">
+        <v>100000</v>
+      </c>
+      <c r="O4">
+        <v>100000</v>
+      </c>
+      <c r="P4">
+        <v>100000</v>
+      </c>
+      <c r="Q4">
+        <v>100000</v>
+      </c>
+      <c r="R4">
+        <v>100000</v>
+      </c>
+      <c r="S4">
+        <v>100000</v>
+      </c>
+      <c r="T4">
+        <v>100000</v>
+      </c>
+      <c r="U4">
+        <v>100000</v>
+      </c>
+      <c r="V4">
+        <v>100000</v>
+      </c>
+      <c r="W4">
+        <v>100000</v>
+      </c>
+      <c r="X4">
+        <v>100000</v>
+      </c>
+      <c r="Y4">
+        <v>100000</v>
+      </c>
+      <c r="Z4">
+        <v>100000</v>
+      </c>
+      <c r="AA4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>100000</v>
+      </c>
+      <c r="C5">
+        <v>100000</v>
+      </c>
+      <c r="D5">
+        <v>100000</v>
+      </c>
+      <c r="E5">
+        <v>100000</v>
+      </c>
+      <c r="F5">
+        <v>100000</v>
+      </c>
+      <c r="G5">
+        <v>100000</v>
+      </c>
+      <c r="H5">
+        <v>100000</v>
+      </c>
+      <c r="I5">
+        <v>100000</v>
+      </c>
+      <c r="J5">
+        <v>100000</v>
+      </c>
+      <c r="K5">
+        <v>100000</v>
+      </c>
+      <c r="L5">
+        <v>100000</v>
+      </c>
+      <c r="M5">
+        <v>100000</v>
+      </c>
+      <c r="N5">
+        <v>100000</v>
+      </c>
+      <c r="O5">
+        <v>100000</v>
+      </c>
+      <c r="P5">
+        <v>100000</v>
+      </c>
+      <c r="Q5">
+        <v>100000</v>
+      </c>
+      <c r="R5">
+        <v>100000</v>
+      </c>
+      <c r="S5">
+        <v>100000</v>
+      </c>
+      <c r="T5">
+        <v>100000</v>
+      </c>
+      <c r="U5">
+        <v>100000</v>
+      </c>
+      <c r="V5">
+        <v>100000</v>
+      </c>
+      <c r="W5">
+        <v>100000</v>
+      </c>
+      <c r="X5">
+        <v>100000</v>
+      </c>
+      <c r="Y5">
+        <v>100000</v>
+      </c>
+      <c r="Z5">
+        <v>100000</v>
+      </c>
+      <c r="AA5">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E234AF8D-964B-419F-969D-C9FD34B2C8AE}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -3936,7 +4808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39EC2A4D-93DC-4E45-8627-2A75EDF5181B}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -4471,7 +5343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18CEE6-4CB2-4E28-86E1-E84E657A73A8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -5006,11 +5878,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5339A0-3D98-43CE-86F7-53EF60721306}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -5082,12 +5954,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F464A74C-C8AE-4B5D-B335-B05DB5565181}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5513,15 +6385,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E46CCB1-2754-42FA-B5C9-8DABA83A320C}">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="18" max="18" width="9.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -5608,446 +6483,85 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9059A3E3-467F-433B-AAF0-DA415330A29D}">
-  <dimension ref="A1:AA5"/>
-  <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection sqref="A1:AA1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="27" width="9.796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1">
-        <v>2025</v>
-      </c>
-      <c r="C1">
-        <v>2026</v>
-      </c>
-      <c r="D1">
-        <v>2027</v>
-      </c>
-      <c r="E1">
-        <v>2028</v>
-      </c>
-      <c r="F1">
-        <v>2029</v>
-      </c>
-      <c r="G1">
-        <v>2030</v>
-      </c>
-      <c r="H1">
-        <v>2031</v>
-      </c>
-      <c r="I1">
-        <v>2032</v>
-      </c>
-      <c r="J1">
-        <v>2033</v>
-      </c>
-      <c r="K1">
-        <v>2034</v>
-      </c>
-      <c r="L1">
-        <v>2035</v>
-      </c>
-      <c r="M1">
-        <v>2036</v>
-      </c>
-      <c r="N1">
-        <v>2037</v>
-      </c>
-      <c r="O1">
-        <v>2038</v>
-      </c>
-      <c r="P1">
-        <v>2039</v>
-      </c>
-      <c r="Q1">
-        <v>2040</v>
-      </c>
-      <c r="R1">
-        <v>2041</v>
-      </c>
-      <c r="S1">
-        <v>2042</v>
-      </c>
-      <c r="T1">
-        <v>2043</v>
-      </c>
-      <c r="U1">
-        <v>2044</v>
-      </c>
-      <c r="V1">
-        <v>2045</v>
-      </c>
-      <c r="W1">
-        <v>2046</v>
-      </c>
-      <c r="X1">
-        <v>2047</v>
-      </c>
-      <c r="Y1">
-        <v>2048</v>
-      </c>
-      <c r="Z1">
-        <v>2049</v>
-      </c>
-      <c r="AA1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1.138931802510158</v>
-      </c>
-      <c r="C2" s="5">
-        <v>7.574766115689437</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.67628647507918527</v>
-      </c>
-      <c r="E2" s="5">
-        <v>3.2136905007923797</v>
-      </c>
-      <c r="F2" s="5">
-        <v>5.6365173572880378</v>
-      </c>
-      <c r="G2" s="5">
-        <v>8.23729264578464</v>
-      </c>
-      <c r="H2" s="5">
-        <v>3.9808290290957169</v>
-      </c>
-      <c r="I2" s="5">
-        <v>4.2084362783232425</v>
-      </c>
-      <c r="J2" s="5">
-        <v>2.6547768072885605</v>
-      </c>
-      <c r="K2" s="5">
-        <v>8.6895749145679559</v>
-      </c>
-      <c r="L2" s="5">
-        <v>4.4525335538469051</v>
-      </c>
-      <c r="M2" s="5">
-        <v>3.4468203268875373</v>
-      </c>
-      <c r="N2" s="5">
-        <v>2.4572713271210231</v>
-      </c>
-      <c r="O2" s="5">
-        <v>8.927728792550143</v>
-      </c>
-      <c r="P2" s="5">
-        <v>5.982551937391019</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>7.3819001349795244E-2</v>
-      </c>
-      <c r="R2" s="5">
-        <v>1.9919161958087483</v>
-      </c>
-      <c r="S2" s="5">
-        <v>2.4831770957740105</v>
-      </c>
-      <c r="T2" s="5">
-        <v>9.4001854872220374</v>
-      </c>
-      <c r="U2" s="5">
-        <v>4.3998924386883029</v>
-      </c>
-      <c r="V2" s="5">
-        <v>0.43428856551232409</v>
-      </c>
-      <c r="W2" s="5">
-        <v>7.9407731237710166</v>
-      </c>
-      <c r="X2" s="5">
-        <v>4.1007272303399853</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>5.8292407312736536</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>0.26933124855980206</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>6.9076528786362008</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1.2044835146641231</v>
-      </c>
-      <c r="C3" s="5">
-        <v>7.987902585292554</v>
-      </c>
-      <c r="D3" s="5">
-        <v>7.9590068482088627</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.1606066383802518</v>
-      </c>
-      <c r="F3" s="5">
-        <v>4.585605094215504</v>
-      </c>
-      <c r="G3" s="5">
-        <v>9.6626632527953404</v>
-      </c>
-      <c r="H3" s="5">
-        <v>5.7739880052029147</v>
-      </c>
-      <c r="I3" s="5">
-        <v>9.2566527937944265</v>
-      </c>
-      <c r="J3" s="5">
-        <v>9.4800396741663029</v>
-      </c>
-      <c r="K3" s="5">
-        <v>3.6065083788586447</v>
-      </c>
-      <c r="L3" s="5">
-        <v>8.5438796497736664</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0.59728548866735287</v>
-      </c>
-      <c r="N3" s="5">
-        <v>3.8461224682055359</v>
-      </c>
-      <c r="O3" s="5">
-        <v>6.6481529824524479</v>
-      </c>
-      <c r="P3" s="5">
-        <v>7.3392403143414278</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>3.1816087694142494</v>
-      </c>
-      <c r="R3" s="5">
-        <v>2.7863956935330956</v>
-      </c>
-      <c r="S3" s="5">
-        <v>9.3348757795029993</v>
-      </c>
-      <c r="T3" s="5">
-        <v>2.1397729972070723</v>
-      </c>
-      <c r="U3" s="5">
-        <v>6.9678153416583575</v>
-      </c>
-      <c r="V3" s="5">
-        <v>7.7674217492321507</v>
-      </c>
-      <c r="W3" s="5">
-        <v>4.7216654236148514</v>
-      </c>
-      <c r="X3" s="5">
-        <v>4.238810750971469</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>7.3608683858912185</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>7.5148932206900243</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>9.6339470176296054</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1.6561115100472845</v>
-      </c>
-      <c r="C4" s="5">
-        <v>6.8203698630888576</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.4137603139272703</v>
-      </c>
-      <c r="E4" s="5">
-        <v>4.3586868316947838</v>
-      </c>
-      <c r="F4" s="5">
-        <v>9.5169563479933696</v>
-      </c>
-      <c r="G4" s="5">
-        <v>6.6592244131241145</v>
-      </c>
-      <c r="H4" s="5">
-        <v>3.2346583782178726</v>
-      </c>
-      <c r="I4" s="5">
-        <v>8.4298844355731966</v>
-      </c>
-      <c r="J4" s="5">
-        <v>2.0837137856376531E-2</v>
-      </c>
-      <c r="K4" s="5">
-        <v>7.801618608794608</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1.1747432563255356</v>
-      </c>
-      <c r="M4" s="5">
-        <v>9.2189855539967063</v>
-      </c>
-      <c r="N4" s="5">
-        <v>5.6389770014244593</v>
-      </c>
-      <c r="O4" s="5">
-        <v>9.3557448426025598</v>
-      </c>
-      <c r="P4" s="5">
-        <v>2.5307863577058676</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>1.8798425218320436</v>
-      </c>
-      <c r="R4" s="5">
-        <v>4.9777650025283062</v>
-      </c>
-      <c r="S4" s="5">
-        <v>2.470635282434567</v>
-      </c>
-      <c r="T4" s="5">
-        <v>8.3448632095880253</v>
-      </c>
-      <c r="U4" s="5">
-        <v>2.8797087757874475</v>
-      </c>
-      <c r="V4" s="5">
-        <v>4.8495072111122131</v>
-      </c>
-      <c r="W4" s="5">
-        <v>0.6494650243068445</v>
-      </c>
-      <c r="X4" s="5">
-        <v>4.0400013877281555</v>
-      </c>
-      <c r="Y4" s="5">
-        <v>8.7109696253244202</v>
-      </c>
-      <c r="Z4" s="5">
-        <v>2.5086878384546196</v>
-      </c>
-      <c r="AA4" s="5">
-        <v>1.6351143304444082</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>9.0280272949077336</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.79148016981419489</v>
-      </c>
-      <c r="D5" s="5">
-        <v>9.3450116579607538</v>
-      </c>
-      <c r="E5" s="5">
-        <v>8.7779321350987356</v>
-      </c>
-      <c r="F5" s="5">
-        <v>9.9122391981291731</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1.6940251254577043</v>
-      </c>
-      <c r="H5" s="5">
-        <v>5.3580360106324925</v>
-      </c>
-      <c r="I5" s="5">
-        <v>2.9089999765545471</v>
-      </c>
-      <c r="J5" s="5">
-        <v>6.3392393508409226</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1.3233246022872935</v>
-      </c>
-      <c r="L5" s="5">
-        <v>1.120067870198912</v>
-      </c>
-      <c r="M5" s="5">
-        <v>7.6992979145058449</v>
-      </c>
-      <c r="N5" s="5">
-        <v>2.5057427861077572</v>
-      </c>
-      <c r="O5" s="5">
-        <v>7.3750450434362538</v>
-      </c>
-      <c r="P5" s="5">
-        <v>9.4007626187483222</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>9.101036356582326E-2</v>
-      </c>
-      <c r="R5" s="5">
-        <v>0.57288500630638395</v>
-      </c>
-      <c r="S5" s="5">
-        <v>7.4626065943311914</v>
-      </c>
-      <c r="T5" s="5">
-        <v>3.1809862851226445</v>
-      </c>
-      <c r="U5" s="5">
-        <v>9.2020936906236397</v>
-      </c>
-      <c r="V5" s="5">
-        <v>7.2239084732453938</v>
-      </c>
-      <c r="W5" s="5">
-        <v>4.8200977144393988</v>
-      </c>
-      <c r="X5" s="5">
-        <v>0.51573154632642448</v>
-      </c>
-      <c r="Y5" s="5">
-        <v>2.0417983331255551</v>
-      </c>
-      <c r="Z5" s="5">
-        <v>4.1086422921963939</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>4.5570832737185842</v>
+        <v>51</v>
+      </c>
+      <c r="B2">
+        <v>500000</v>
+      </c>
+      <c r="C2">
+        <v>500000</v>
+      </c>
+      <c r="D2">
+        <v>500000</v>
+      </c>
+      <c r="E2">
+        <v>500000</v>
+      </c>
+      <c r="F2">
+        <v>500000</v>
+      </c>
+      <c r="G2">
+        <v>500000</v>
+      </c>
+      <c r="H2">
+        <v>500000</v>
+      </c>
+      <c r="I2">
+        <v>500000</v>
+      </c>
+      <c r="J2">
+        <v>500000</v>
+      </c>
+      <c r="K2">
+        <v>500000</v>
+      </c>
+      <c r="L2">
+        <v>500000</v>
+      </c>
+      <c r="M2">
+        <v>500000</v>
+      </c>
+      <c r="N2">
+        <v>500000</v>
+      </c>
+      <c r="O2">
+        <v>500000</v>
+      </c>
+      <c r="P2">
+        <v>500000</v>
+      </c>
+      <c r="Q2">
+        <v>500000</v>
+      </c>
+      <c r="R2">
+        <v>500000</v>
+      </c>
+      <c r="S2">
+        <v>500000</v>
+      </c>
+      <c r="T2">
+        <v>500000</v>
+      </c>
+      <c r="U2">
+        <v>500000</v>
+      </c>
+      <c r="V2">
+        <v>500000</v>
+      </c>
+      <c r="W2">
+        <v>500000</v>
+      </c>
+      <c r="X2">
+        <v>500000</v>
+      </c>
+      <c r="Y2">
+        <v>500000</v>
+      </c>
+      <c r="Z2">
+        <v>500000</v>
+      </c>
+      <c r="AA2">
+        <v>500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. steel_pathway_v0.1_ClearnSystemWide 2. steel_pathway_v0.1_emission_multifuel
</commit_message>
<xml_diff>
--- a/database/steel_data.xlsx
+++ b/database/steel_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PLANiT\github\macc_steel\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365BA471-2FC7-4789-8419-BDA75AEC4FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC535C40-6C13-4C5E-8B4C-771971B3DB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="348" windowWidth="28620" windowHeight="12264" tabRatio="620" activeTab="6" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
+    <workbookView xWindow="204" yWindow="348" windowWidth="28620" windowHeight="12264" tabRatio="620" activeTab="2" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="18" r:id="rId1"/>
@@ -3985,8 +3985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E683ACB1-236C-41D9-AD28-376C61929EF9}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:AA3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4082,82 +4082,82 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>10000000</v>
+        <v>1500000</v>
       </c>
       <c r="C2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="D2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="E2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="F2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="G2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="H2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="I2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="J2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="K2">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="L2">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="M2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="N2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="O2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="P2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="Q2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="R2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="S2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="T2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="U2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="V2">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>100000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
@@ -4165,82 +4165,82 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="C3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="D3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="E3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="F3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="G3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="H3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="I3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="J3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="K3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="L3">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="M3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="N3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="O3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="P3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="Q3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="R3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="S3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="T3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="U3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="V3">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <v>100000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -4308,7 +4308,7 @@
         <v>50000</v>
       </c>
       <c r="V4">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -4391,7 +4391,7 @@
         <v>50000</v>
       </c>
       <c r="V5">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -5946,8 +5946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5339A0-3D98-43CE-86F7-53EF60721306}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6454,7 +6454,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:AA2"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6611,22 +6611,22 @@
         <v>10000000</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean System Level v0.1
</commit_message>
<xml_diff>
--- a/database/steel_data.xlsx
+++ b/database/steel_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PLANiT\github\macc_steel\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC535C40-6C13-4C5E-8B4C-771971B3DB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07AE055-EB32-4A37-AB8E-21D4E2AA2CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="348" windowWidth="28620" windowHeight="12264" tabRatio="620" activeTab="2" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
+    <workbookView xWindow="1644" yWindow="804" windowWidth="43116" windowHeight="20856" tabRatio="620" activeTab="2" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="18" r:id="rId1"/>
@@ -669,10 +669,14 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
@@ -778,10 +782,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9059A3E3-467F-433B-AAF0-DA415330A29D}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection sqref="A1:AA1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -877,82 +881,82 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>1.138931802510158</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>7.574766115689437</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5">
-        <v>0.67628647507918527</v>
+        <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>3.2136905007923797</v>
+        <v>1</v>
       </c>
       <c r="F2" s="5">
-        <v>5.6365173572880378</v>
+        <v>1</v>
       </c>
       <c r="G2" s="5">
-        <v>8.23729264578464</v>
+        <v>1</v>
       </c>
       <c r="H2" s="5">
-        <v>3.9808290290957169</v>
+        <v>1</v>
       </c>
       <c r="I2" s="5">
-        <v>4.2084362783232425</v>
+        <v>1</v>
       </c>
       <c r="J2" s="5">
-        <v>2.6547768072885605</v>
+        <v>1</v>
       </c>
       <c r="K2" s="5">
-        <v>8.6895749145679559</v>
+        <v>1</v>
       </c>
       <c r="L2" s="5">
-        <v>4.4525335538469051</v>
+        <v>1</v>
       </c>
       <c r="M2" s="5">
-        <v>3.4468203268875373</v>
+        <v>1</v>
       </c>
       <c r="N2" s="5">
-        <v>2.4572713271210231</v>
+        <v>1</v>
       </c>
       <c r="O2" s="5">
-        <v>8.927728792550143</v>
+        <v>1</v>
       </c>
       <c r="P2" s="5">
-        <v>5.982551937391019</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="5">
-        <v>7.3819001349795244E-2</v>
+        <v>1</v>
       </c>
       <c r="R2" s="5">
-        <v>1.9919161958087483</v>
+        <v>1</v>
       </c>
       <c r="S2" s="5">
-        <v>2.4831770957740105</v>
+        <v>1</v>
       </c>
       <c r="T2" s="5">
-        <v>9.4001854872220374</v>
+        <v>1</v>
       </c>
       <c r="U2" s="5">
-        <v>4.3998924386883029</v>
+        <v>1</v>
       </c>
       <c r="V2" s="5">
-        <v>0.43428856551232409</v>
+        <v>1</v>
       </c>
       <c r="W2" s="5">
-        <v>7.9407731237710166</v>
+        <v>1</v>
       </c>
       <c r="X2" s="5">
-        <v>4.1007272303399853</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="5">
-        <v>5.8292407312736536</v>
+        <v>1</v>
       </c>
       <c r="Z2" s="5">
-        <v>0.26933124855980206</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="5">
-        <v>6.9076528786362008</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
@@ -960,82 +964,82 @@
         <v>10</v>
       </c>
       <c r="B3" s="5">
-        <v>1.2044835146641231</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5">
-        <v>7.987902585292554</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5">
-        <v>7.9590068482088627</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5">
-        <v>0.1606066383802518</v>
+        <v>8</v>
       </c>
       <c r="F3" s="5">
-        <v>4.585605094215504</v>
+        <v>8</v>
       </c>
       <c r="G3" s="5">
-        <v>9.6626632527953404</v>
+        <v>8</v>
       </c>
       <c r="H3" s="5">
-        <v>5.7739880052029147</v>
+        <v>8</v>
       </c>
       <c r="I3" s="5">
-        <v>9.2566527937944265</v>
+        <v>8</v>
       </c>
       <c r="J3" s="5">
-        <v>9.4800396741663029</v>
+        <v>8</v>
       </c>
       <c r="K3" s="5">
-        <v>3.6065083788586447</v>
+        <v>8</v>
       </c>
       <c r="L3" s="5">
-        <v>8.5438796497736664</v>
+        <v>8</v>
       </c>
       <c r="M3" s="5">
-        <v>0.59728548866735287</v>
+        <v>8</v>
       </c>
       <c r="N3" s="5">
-        <v>3.8461224682055359</v>
+        <v>8</v>
       </c>
       <c r="O3" s="5">
-        <v>6.6481529824524479</v>
+        <v>8</v>
       </c>
       <c r="P3" s="5">
-        <v>7.3392403143414278</v>
+        <v>8</v>
       </c>
       <c r="Q3" s="5">
-        <v>3.1816087694142494</v>
+        <v>8</v>
       </c>
       <c r="R3" s="5">
-        <v>2.7863956935330956</v>
+        <v>8</v>
       </c>
       <c r="S3" s="5">
-        <v>9.3348757795029993</v>
+        <v>8</v>
       </c>
       <c r="T3" s="5">
-        <v>2.1397729972070723</v>
+        <v>8</v>
       </c>
       <c r="U3" s="5">
-        <v>6.9678153416583575</v>
+        <v>8</v>
       </c>
       <c r="V3" s="5">
-        <v>7.7674217492321507</v>
+        <v>8</v>
       </c>
       <c r="W3" s="5">
-        <v>4.7216654236148514</v>
+        <v>8</v>
       </c>
       <c r="X3" s="5">
-        <v>4.238810750971469</v>
+        <v>8</v>
       </c>
       <c r="Y3" s="5">
-        <v>7.3608683858912185</v>
+        <v>8</v>
       </c>
       <c r="Z3" s="5">
-        <v>7.5148932206900243</v>
+        <v>8</v>
       </c>
       <c r="AA3" s="5">
-        <v>9.6339470176296054</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -1043,82 +1047,82 @@
         <v>11</v>
       </c>
       <c r="B4" s="5">
-        <v>1.6561115100472845</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5">
-        <v>6.8203698630888576</v>
+        <v>10</v>
       </c>
       <c r="D4" s="5">
-        <v>1.4137603139272703</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5">
-        <v>4.3586868316947838</v>
+        <v>10</v>
       </c>
       <c r="F4" s="5">
-        <v>9.5169563479933696</v>
+        <v>10</v>
       </c>
       <c r="G4" s="5">
-        <v>6.6592244131241145</v>
+        <v>10</v>
       </c>
       <c r="H4" s="5">
-        <v>3.2346583782178726</v>
+        <v>10</v>
       </c>
       <c r="I4" s="5">
-        <v>8.4298844355731966</v>
+        <v>10</v>
       </c>
       <c r="J4" s="5">
-        <v>2.0837137856376531E-2</v>
+        <v>10</v>
       </c>
       <c r="K4" s="5">
-        <v>7.801618608794608</v>
+        <v>10</v>
       </c>
       <c r="L4" s="5">
-        <v>1.1747432563255356</v>
+        <v>10</v>
       </c>
       <c r="M4" s="5">
-        <v>9.2189855539967063</v>
+        <v>10</v>
       </c>
       <c r="N4" s="5">
-        <v>5.6389770014244593</v>
+        <v>10</v>
       </c>
       <c r="O4" s="5">
-        <v>9.3557448426025598</v>
+        <v>10</v>
       </c>
       <c r="P4" s="5">
-        <v>2.5307863577058676</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="5">
-        <v>1.8798425218320436</v>
+        <v>10</v>
       </c>
       <c r="R4" s="5">
-        <v>4.9777650025283062</v>
+        <v>10</v>
       </c>
       <c r="S4" s="5">
-        <v>2.470635282434567</v>
+        <v>10</v>
       </c>
       <c r="T4" s="5">
-        <v>8.3448632095880253</v>
+        <v>10</v>
       </c>
       <c r="U4" s="5">
-        <v>2.8797087757874475</v>
+        <v>10</v>
       </c>
       <c r="V4" s="5">
-        <v>4.8495072111122131</v>
+        <v>10</v>
       </c>
       <c r="W4" s="5">
-        <v>0.6494650243068445</v>
+        <v>10</v>
       </c>
       <c r="X4" s="5">
-        <v>4.0400013877281555</v>
+        <v>10</v>
       </c>
       <c r="Y4" s="5">
-        <v>8.7109696253244202</v>
+        <v>10</v>
       </c>
       <c r="Z4" s="5">
-        <v>2.5086878384546196</v>
+        <v>10</v>
       </c>
       <c r="AA4" s="5">
-        <v>1.6351143304444082</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.4">
@@ -1126,83 +1130,112 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>9.0280272949077336</v>
+        <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>0.79148016981419489</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5">
-        <v>9.3450116579607538</v>
+        <v>5</v>
       </c>
       <c r="E5" s="5">
-        <v>8.7779321350987356</v>
+        <v>5</v>
       </c>
       <c r="F5" s="5">
-        <v>9.9122391981291731</v>
+        <v>5</v>
       </c>
       <c r="G5" s="5">
-        <v>1.6940251254577043</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="5">
-        <v>5.3580360106324925</v>
+        <v>0.5</v>
       </c>
       <c r="I5" s="5">
-        <v>2.9089999765545471</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="5">
-        <v>6.3392393508409226</v>
+        <v>0.5</v>
       </c>
       <c r="K5" s="5">
-        <v>1.3233246022872935</v>
+        <v>0.5</v>
       </c>
       <c r="L5" s="5">
-        <v>1.120067870198912</v>
+        <v>0.5</v>
       </c>
       <c r="M5" s="5">
-        <v>7.6992979145058449</v>
+        <v>0.5</v>
       </c>
       <c r="N5" s="5">
-        <v>2.5057427861077572</v>
+        <v>0.5</v>
       </c>
       <c r="O5" s="5">
-        <v>7.3750450434362538</v>
+        <v>0.5</v>
       </c>
       <c r="P5" s="5">
-        <v>9.4007626187483222</v>
+        <v>0.5</v>
       </c>
       <c r="Q5" s="5">
-        <v>9.101036356582326E-2</v>
+        <v>0.5</v>
       </c>
       <c r="R5" s="5">
-        <v>0.57288500630638395</v>
+        <v>0.5</v>
       </c>
       <c r="S5" s="5">
-        <v>7.4626065943311914</v>
+        <v>0.5</v>
       </c>
       <c r="T5" s="5">
-        <v>3.1809862851226445</v>
+        <v>0.5</v>
       </c>
       <c r="U5" s="5">
-        <v>9.2020936906236397</v>
+        <v>0.5</v>
       </c>
       <c r="V5" s="5">
-        <v>7.2239084732453938</v>
+        <v>0.5</v>
       </c>
       <c r="W5" s="5">
-        <v>4.8200977144393988</v>
+        <v>0.5</v>
       </c>
       <c r="X5" s="5">
-        <v>0.51573154632642448</v>
+        <v>0.5</v>
       </c>
       <c r="Y5" s="5">
-        <v>2.0417983331255551</v>
+        <v>0.5</v>
       </c>
       <c r="Z5" s="5">
-        <v>4.1086422921963939</v>
+        <v>0.5</v>
       </c>
       <c r="AA5" s="5">
-        <v>4.5570832737185842</v>
-      </c>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1212,15 +1245,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E18AD-1C92-4B5C-962D-792F4AC09175}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AA5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="27" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="27" width="9.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
@@ -1394,82 +1428,82 @@
         <v>10</v>
       </c>
       <c r="B3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -1477,82 +1511,82 @@
         <v>11</v>
       </c>
       <c r="B4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.4">
@@ -1560,83 +1594,112 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="5">
-        <v>3</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1646,9 +1709,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CF035B-C14B-46B7-A841-579E94220A37}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -1989,83 +2054,112 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="F5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="G5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="J5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="L5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="M5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="N5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="O5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="P5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="R5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="S5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="T5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="U5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="V5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="W5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="X5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="Y5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="AA5" s="5">
-        <v>1.1000000000000001</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2078,7 +2172,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2116,7 +2210,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -2127,7 +2221,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -2149,7 +2243,7 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -2171,7 +2265,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -2193,7 +2287,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2207,10 +2301,13 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
@@ -2275,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -2322,7 +2419,7 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AA1"/>
+      <selection activeCell="B2" sqref="B2:AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2415,82 +2512,82 @@
         <v>5</v>
       </c>
       <c r="B2" s="5">
-        <v>1.138931802510158</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>7.574766115689437</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5">
-        <v>0.67628647507918527</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
-        <v>3.2136905007923797</v>
+        <v>0</v>
       </c>
       <c r="F2" s="5">
-        <v>5.6365173572880378</v>
+        <v>0</v>
       </c>
       <c r="G2" s="5">
-        <v>8.23729264578464</v>
+        <v>0</v>
       </c>
       <c r="H2" s="5">
-        <v>3.9808290290957169</v>
+        <v>0</v>
       </c>
       <c r="I2" s="5">
-        <v>4.2084362783232425</v>
+        <v>0</v>
       </c>
       <c r="J2" s="5">
-        <v>2.6547768072885605</v>
+        <v>0</v>
       </c>
       <c r="K2" s="5">
-        <v>8.6895749145679559</v>
+        <v>0</v>
       </c>
       <c r="L2" s="5">
-        <v>4.4525335538469051</v>
+        <v>0</v>
       </c>
       <c r="M2" s="5">
-        <v>3.4468203268875373</v>
+        <v>0</v>
       </c>
       <c r="N2" s="5">
-        <v>2.4572713271210231</v>
+        <v>0</v>
       </c>
       <c r="O2" s="5">
-        <v>8.927728792550143</v>
+        <v>0</v>
       </c>
       <c r="P2" s="5">
-        <v>5.982551937391019</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="5">
-        <v>7.3819001349795244E-2</v>
+        <v>0</v>
       </c>
       <c r="R2" s="5">
-        <v>1.9919161958087483</v>
+        <v>0</v>
       </c>
       <c r="S2" s="5">
-        <v>2.4831770957740105</v>
+        <v>0</v>
       </c>
       <c r="T2" s="5">
-        <v>9.4001854872220374</v>
+        <v>0</v>
       </c>
       <c r="U2" s="5">
-        <v>4.3998924386883029</v>
+        <v>0</v>
       </c>
       <c r="V2" s="5">
-        <v>0.43428856551232409</v>
+        <v>0</v>
       </c>
       <c r="W2" s="5">
-        <v>7.9407731237710166</v>
+        <v>0</v>
       </c>
       <c r="X2" s="5">
-        <v>4.1007272303399853</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="5">
-        <v>5.8292407312736536</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="5">
-        <v>0.26933124855980206</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="5">
-        <v>6.9076528786362008</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
@@ -2498,82 +2595,82 @@
         <v>6</v>
       </c>
       <c r="B3" s="5">
-        <v>1.2044835146641231</v>
+        <v>2</v>
       </c>
       <c r="C3" s="5">
-        <v>7.987902585292554</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5">
-        <v>7.9590068482088627</v>
+        <v>2</v>
       </c>
       <c r="E3" s="5">
-        <v>0.1606066383802518</v>
+        <v>2</v>
       </c>
       <c r="F3" s="5">
-        <v>4.585605094215504</v>
+        <v>2</v>
       </c>
       <c r="G3" s="5">
-        <v>9.6626632527953404</v>
+        <v>2</v>
       </c>
       <c r="H3" s="5">
-        <v>5.7739880052029147</v>
+        <v>2</v>
       </c>
       <c r="I3" s="5">
-        <v>9.2566527937944265</v>
+        <v>2</v>
       </c>
       <c r="J3" s="5">
-        <v>9.4800396741663029</v>
+        <v>2</v>
       </c>
       <c r="K3" s="5">
-        <v>3.6065083788586447</v>
+        <v>2</v>
       </c>
       <c r="L3" s="5">
-        <v>8.5438796497736664</v>
+        <v>2</v>
       </c>
       <c r="M3" s="5">
-        <v>0.59728548866735287</v>
+        <v>2</v>
       </c>
       <c r="N3" s="5">
-        <v>3.8461224682055359</v>
+        <v>2</v>
       </c>
       <c r="O3" s="5">
-        <v>6.6481529824524479</v>
+        <v>2</v>
       </c>
       <c r="P3" s="5">
-        <v>7.3392403143414278</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="5">
-        <v>3.1816087694142494</v>
+        <v>2</v>
       </c>
       <c r="R3" s="5">
-        <v>2.7863956935330956</v>
+        <v>2</v>
       </c>
       <c r="S3" s="5">
-        <v>9.3348757795029993</v>
+        <v>2</v>
       </c>
       <c r="T3" s="5">
-        <v>2.1397729972070723</v>
+        <v>2</v>
       </c>
       <c r="U3" s="5">
-        <v>6.9678153416583575</v>
+        <v>2</v>
       </c>
       <c r="V3" s="5">
-        <v>7.7674217492321507</v>
+        <v>2</v>
       </c>
       <c r="W3" s="5">
-        <v>4.7216654236148514</v>
+        <v>2</v>
       </c>
       <c r="X3" s="5">
-        <v>4.238810750971469</v>
+        <v>2</v>
       </c>
       <c r="Y3" s="5">
-        <v>7.3608683858912185</v>
+        <v>2</v>
       </c>
       <c r="Z3" s="5">
-        <v>7.5148932206900243</v>
+        <v>2</v>
       </c>
       <c r="AA3" s="5">
-        <v>9.6339470176296054</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -2581,82 +2678,82 @@
         <v>7</v>
       </c>
       <c r="B4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="O4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="P4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Q4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="R4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="S4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="T4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="U4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="V4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="W4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="X4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Y4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Z4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AA4" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.4">
@@ -2664,82 +2761,82 @@
         <v>8</v>
       </c>
       <c r="B5" s="5">
-        <v>9.0280272949077336</v>
+        <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>0.79148016981419489</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5">
-        <v>9.3450116579607538</v>
+        <v>5</v>
       </c>
       <c r="E5" s="5">
-        <v>8.7779321350987356</v>
+        <v>5</v>
       </c>
       <c r="F5" s="5">
-        <v>9.9122391981291731</v>
+        <v>5</v>
       </c>
       <c r="G5" s="5">
-        <v>1.6940251254577043</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="5">
-        <v>5.3580360106324925</v>
+        <v>0.5</v>
       </c>
       <c r="I5" s="5">
-        <v>2.9089999765545471</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="5">
-        <v>6.3392393508409226</v>
+        <v>0.5</v>
       </c>
       <c r="K5" s="5">
-        <v>1.3233246022872935</v>
+        <v>0.5</v>
       </c>
       <c r="L5" s="5">
-        <v>1.120067870198912</v>
+        <v>0.5</v>
       </c>
       <c r="M5" s="5">
-        <v>7.6992979145058449</v>
+        <v>0.5</v>
       </c>
       <c r="N5" s="5">
-        <v>2.5057427861077572</v>
+        <v>0.5</v>
       </c>
       <c r="O5" s="5">
-        <v>7.3750450434362538</v>
+        <v>0.5</v>
       </c>
       <c r="P5" s="5">
-        <v>9.4007626187483222</v>
+        <v>0.5</v>
       </c>
       <c r="Q5" s="5">
-        <v>9.101036356582326E-2</v>
+        <v>0.5</v>
       </c>
       <c r="R5" s="5">
-        <v>0.57288500630638395</v>
+        <v>0.5</v>
       </c>
       <c r="S5" s="5">
-        <v>7.4626065943311914</v>
+        <v>0.5</v>
       </c>
       <c r="T5" s="5">
-        <v>3.1809862851226445</v>
+        <v>0.5</v>
       </c>
       <c r="U5" s="5">
-        <v>9.2020936906236397</v>
+        <v>0.5</v>
       </c>
       <c r="V5" s="5">
-        <v>7.2239084732453938</v>
+        <v>0.5</v>
       </c>
       <c r="W5" s="5">
-        <v>4.8200977144393988</v>
+        <v>0.5</v>
       </c>
       <c r="X5" s="5">
-        <v>0.51573154632642448</v>
+        <v>0.5</v>
       </c>
       <c r="Y5" s="5">
-        <v>2.0417983331255551</v>
+        <v>0.5</v>
       </c>
       <c r="Z5" s="5">
-        <v>4.1086422921963939</v>
+        <v>0.5</v>
       </c>
       <c r="AA5" s="5">
-        <v>4.5570832737185842</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.4">
@@ -2747,82 +2844,82 @@
         <v>9</v>
       </c>
       <c r="B6" s="5">
-        <v>7.8957032192905761</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5">
-        <v>4.6082787714867699</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5">
-        <v>0.6091916868338465</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5">
-        <v>4.5793589856973238</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5">
-        <v>8.1786077617116337</v>
+        <v>7</v>
       </c>
       <c r="G6" s="5">
-        <v>8.0194570739747864</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="5">
-        <v>5.3363776828222846</v>
+        <v>0.5</v>
       </c>
       <c r="I6" s="5">
-        <v>2.0392354662996173</v>
+        <v>0.5</v>
       </c>
       <c r="J6" s="5">
-        <v>1.5611429793634013</v>
+        <v>0.5</v>
       </c>
       <c r="K6" s="5">
-        <v>4.8911639936651881</v>
+        <v>0.5</v>
       </c>
       <c r="L6" s="5">
-        <v>0.40969313950629416</v>
+        <v>0.5</v>
       </c>
       <c r="M6" s="5">
-        <v>8.1821714040505622</v>
+        <v>0.5</v>
       </c>
       <c r="N6" s="5">
-        <v>7.1594690363400781</v>
+        <v>0.5</v>
       </c>
       <c r="O6" s="5">
-        <v>9.6385261152701958</v>
+        <v>0.5</v>
       </c>
       <c r="P6" s="5">
-        <v>6.1105005430337744</v>
+        <v>0.5</v>
       </c>
       <c r="Q6" s="5">
-        <v>9.8360503707220346</v>
+        <v>0.5</v>
       </c>
       <c r="R6" s="5">
-        <v>3.1687053337959927</v>
+        <v>0.5</v>
       </c>
       <c r="S6" s="5">
-        <v>7.4574597903735853</v>
+        <v>0.5</v>
       </c>
       <c r="T6" s="5">
-        <v>1.7179916959018882</v>
+        <v>0.5</v>
       </c>
       <c r="U6" s="5">
-        <v>1.3703096017555394</v>
+        <v>0.5</v>
       </c>
       <c r="V6" s="5">
-        <v>1.224292525245001</v>
+        <v>0.5</v>
       </c>
       <c r="W6" s="5">
-        <v>9.9777665023046573</v>
+        <v>0.5</v>
       </c>
       <c r="X6" s="5">
-        <v>0.23044312727864225</v>
+        <v>0.5</v>
       </c>
       <c r="Y6" s="5">
-        <v>4.2498432589860649</v>
+        <v>0.5</v>
       </c>
       <c r="Z6" s="5">
-        <v>0.66055919821920162</v>
+        <v>0.5</v>
       </c>
       <c r="AA6" s="5">
-        <v>5.425378034772347</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -3350,7 +3447,7 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3864,7 +3961,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3912,7 +4009,7 @@
         <v>4000</v>
       </c>
       <c r="F2">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -3929,17 +4026,17 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="F3">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -3949,17 +4046,17 @@
         <v>21</v>
       </c>
       <c r="E4">
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="F4">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -3969,10 +4066,10 @@
         <v>21</v>
       </c>
       <c r="E5">
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="F5">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
   </sheetData>
@@ -3985,8 +4082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E683ACB1-236C-41D9-AD28-376C61929EF9}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:AA2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4082,34 +4179,34 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>1500000</v>
+        <v>99999999</v>
       </c>
       <c r="C2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="D2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="E2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="F2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="G2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="H2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="I2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="J2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="K2">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="L2">
         <v>1000000</v>
@@ -4142,22 +4239,22 @@
         <v>1000000</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
@@ -4165,7 +4262,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>1000000</v>
+        <v>99999999</v>
       </c>
       <c r="C3">
         <v>1000000</v>
@@ -4225,22 +4322,22 @@
         <v>1000000</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -4248,82 +4345,82 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>50000</v>
+        <v>99999999</v>
       </c>
       <c r="C4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="D4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="E4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="F4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="G4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="H4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="I4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="J4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="K4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="L4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="M4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="O4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="P4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="Q4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="R4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="S4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="T4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="U4">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.4">
@@ -4331,82 +4428,82 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>50000</v>
+        <v>99999999</v>
       </c>
       <c r="C5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="D5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="E5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="F5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="G5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="H5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="I5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="J5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="K5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="L5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="M5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="O5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="P5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="Q5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="R5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="S5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="T5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="U5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -4420,7 +4517,7 @@
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="Q3" sqref="Q3:AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4513,82 +4610,82 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="H2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="I2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="J2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="K2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="L2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="M2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="N2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="O2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="P2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="Q2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="R2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="S2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="T2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="U2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="V2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="W2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="X2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="Y2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="Z2">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="AA2">
-        <v>30</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
@@ -4596,82 +4693,82 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>150</v>
+        <v>9000</v>
       </c>
       <c r="C3" s="4">
-        <v>145.33333333333331</v>
+        <v>9000</v>
       </c>
       <c r="D3" s="4">
-        <v>140.66666666666666</v>
+        <v>9000</v>
       </c>
       <c r="E3" s="4">
-        <v>136</v>
+        <v>9000</v>
       </c>
       <c r="F3" s="4">
-        <v>131.33333333333334</v>
+        <v>9000</v>
       </c>
       <c r="G3" s="4">
-        <v>126.66666666666666</v>
+        <v>9000</v>
       </c>
       <c r="H3" s="4">
-        <v>122</v>
+        <v>9000</v>
       </c>
       <c r="I3" s="4">
-        <v>117.33333333333334</v>
+        <v>9000</v>
       </c>
       <c r="J3" s="4">
-        <v>112.66666666666667</v>
+        <v>9000</v>
       </c>
       <c r="K3" s="4">
-        <v>108</v>
+        <v>9000</v>
       </c>
       <c r="L3" s="4">
-        <v>103.33333333333334</v>
+        <v>300</v>
       </c>
       <c r="M3" s="4">
-        <v>98.666666666666671</v>
+        <v>300</v>
       </c>
       <c r="N3" s="4">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="O3" s="4">
-        <v>40</v>
+        <v>300</v>
       </c>
       <c r="P3" s="4">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="Q3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="V3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="X3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Z3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AA3" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -4679,82 +4776,82 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>4500</v>
       </c>
       <c r="C4">
-        <v>79</v>
+        <v>4500</v>
       </c>
       <c r="D4">
-        <v>78</v>
+        <v>4500</v>
       </c>
       <c r="E4">
-        <v>77</v>
+        <v>4500</v>
       </c>
       <c r="F4">
-        <v>76</v>
+        <v>4500</v>
       </c>
       <c r="G4">
-        <v>75</v>
+        <v>4500</v>
       </c>
       <c r="H4">
-        <v>74</v>
+        <v>4500</v>
       </c>
       <c r="I4">
-        <v>73</v>
+        <v>4500</v>
       </c>
       <c r="J4">
-        <v>72</v>
+        <v>4500</v>
       </c>
       <c r="K4">
-        <v>71</v>
+        <v>4500</v>
       </c>
       <c r="L4">
-        <v>70</v>
+        <v>4500</v>
       </c>
       <c r="M4">
-        <v>69</v>
+        <v>4500</v>
       </c>
       <c r="N4">
-        <v>68</v>
+        <v>4500</v>
       </c>
       <c r="O4">
-        <v>67</v>
+        <v>4500</v>
       </c>
       <c r="P4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="Q4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="R4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="S4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="T4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="U4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="V4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="W4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="X4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="Y4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="Z4">
-        <v>20</v>
+        <v>4500</v>
       </c>
       <c r="AA4">
-        <v>20</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -4763,107 +4860,107 @@
       </c>
       <c r="B5">
         <f>B2*1.5</f>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:AA5" si="0">C2*1.5</f>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="V5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="W5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="X5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="Y5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
       <c r="AA5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>750</v>
       </c>
     </row>
   </sheetData>
@@ -4971,107 +5068,107 @@
       </c>
       <c r="B2" s="3">
         <f>capex!B2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3">
         <f>capex!C2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3">
         <f>capex!D2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3">
         <f>capex!E2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3">
         <f>capex!F2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3">
         <f>capex!G2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3">
         <f>capex!H2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="I2" s="3">
         <f>capex!I2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="J2" s="3">
         <f>capex!J2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="K2" s="3">
         <f>capex!K2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="L2" s="3">
         <f>capex!L2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="M2" s="3">
         <f>capex!M2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="N2" s="3">
         <f>capex!N2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="O2" s="3">
         <f>capex!O2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="P2" s="3">
         <f>capex!P2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="3">
         <f>capex!Q2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="R2" s="3">
         <f>capex!R2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="S2" s="3">
         <f>capex!S2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="T2" s="3">
         <f>capex!T2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="U2" s="3">
         <f>capex!U2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="V2" s="3">
         <f>capex!V2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="W2" s="3">
         <f>capex!W2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="X2" s="3">
         <f>capex!X2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="Y2" s="3">
         <f>capex!Y2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="Z2" s="3">
         <f>capex!Z2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="AA2" s="3">
         <f>capex!AA2*0.05</f>
-        <v>1.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
@@ -5080,107 +5177,107 @@
       </c>
       <c r="B3" s="3">
         <f>capex!B3*0.05</f>
-        <v>7.5</v>
+        <v>450</v>
       </c>
       <c r="C3" s="3">
         <f>capex!C3*0.05</f>
-        <v>7.2666666666666657</v>
+        <v>450</v>
       </c>
       <c r="D3" s="3">
         <f>capex!D3*0.05</f>
-        <v>7.0333333333333332</v>
+        <v>450</v>
       </c>
       <c r="E3" s="3">
         <f>capex!E3*0.05</f>
-        <v>6.8000000000000007</v>
+        <v>450</v>
       </c>
       <c r="F3" s="3">
         <f>capex!F3*0.05</f>
-        <v>6.5666666666666673</v>
+        <v>450</v>
       </c>
       <c r="G3" s="3">
         <f>capex!G3*0.05</f>
-        <v>6.333333333333333</v>
+        <v>450</v>
       </c>
       <c r="H3" s="3">
         <f>capex!H3*0.05</f>
-        <v>6.1000000000000005</v>
+        <v>450</v>
       </c>
       <c r="I3" s="3">
         <f>capex!I3*0.05</f>
-        <v>5.8666666666666671</v>
+        <v>450</v>
       </c>
       <c r="J3" s="3">
         <f>capex!J3*0.05</f>
-        <v>5.6333333333333337</v>
+        <v>450</v>
       </c>
       <c r="K3" s="3">
         <f>capex!K3*0.05</f>
-        <v>5.4</v>
+        <v>450</v>
       </c>
       <c r="L3" s="3">
         <f>capex!L3*0.05</f>
-        <v>5.1666666666666679</v>
+        <v>15</v>
       </c>
       <c r="M3" s="3">
         <f>capex!M3*0.05</f>
-        <v>4.9333333333333336</v>
+        <v>15</v>
       </c>
       <c r="N3" s="3">
         <f>capex!N3*0.05</f>
-        <v>2.5</v>
+        <v>15</v>
       </c>
       <c r="O3" s="3">
         <f>capex!O3*0.05</f>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="P3" s="3">
         <f>capex!P3*0.05</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="3">
         <f>capex!Q3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R3" s="3">
         <f>capex!R3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S3" s="3">
         <f>capex!S3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T3" s="3">
         <f>capex!T3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U3" s="3">
         <f>capex!U3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V3" s="3">
         <f>capex!V3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W3" s="3">
         <f>capex!W3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X3" s="3">
         <f>capex!X3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y3" s="3">
         <f>capex!Y3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="3">
         <f>capex!Z3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA3" s="3">
         <f>capex!AA3*0.05</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -5189,107 +5286,107 @@
       </c>
       <c r="B4" s="3">
         <f>capex!B4*0.05</f>
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="C4" s="3">
         <f>capex!C4*0.05</f>
-        <v>3.95</v>
+        <v>225</v>
       </c>
       <c r="D4" s="3">
         <f>capex!D4*0.05</f>
-        <v>3.9000000000000004</v>
+        <v>225</v>
       </c>
       <c r="E4" s="3">
         <f>capex!E4*0.05</f>
-        <v>3.85</v>
+        <v>225</v>
       </c>
       <c r="F4" s="3">
         <f>capex!F4*0.05</f>
-        <v>3.8000000000000003</v>
+        <v>225</v>
       </c>
       <c r="G4" s="3">
         <f>capex!G4*0.05</f>
-        <v>3.75</v>
+        <v>225</v>
       </c>
       <c r="H4" s="3">
         <f>capex!H4*0.05</f>
-        <v>3.7</v>
+        <v>225</v>
       </c>
       <c r="I4" s="3">
         <f>capex!I4*0.05</f>
-        <v>3.6500000000000004</v>
+        <v>225</v>
       </c>
       <c r="J4" s="3">
         <f>capex!J4*0.05</f>
-        <v>3.6</v>
+        <v>225</v>
       </c>
       <c r="K4" s="3">
         <f>capex!K4*0.05</f>
-        <v>3.5500000000000003</v>
+        <v>225</v>
       </c>
       <c r="L4" s="3">
         <f>capex!L4*0.05</f>
-        <v>3.5</v>
+        <v>225</v>
       </c>
       <c r="M4" s="3">
         <f>capex!M4*0.05</f>
-        <v>3.45</v>
+        <v>225</v>
       </c>
       <c r="N4" s="3">
         <f>capex!N4*0.05</f>
-        <v>3.4000000000000004</v>
+        <v>225</v>
       </c>
       <c r="O4" s="3">
         <f>capex!O4*0.05</f>
-        <v>3.35</v>
+        <v>225</v>
       </c>
       <c r="P4" s="3">
         <f>capex!P4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="Q4" s="3">
         <f>capex!Q4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="R4" s="3">
         <f>capex!R4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="S4" s="3">
         <f>capex!S4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="T4" s="3">
         <f>capex!T4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="U4" s="3">
         <f>capex!U4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="V4" s="3">
         <f>capex!V4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="W4" s="3">
         <f>capex!W4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="X4" s="3">
         <f>capex!X4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="Y4" s="3">
         <f>capex!Y4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="Z4" s="3">
         <f>capex!Z4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
       <c r="AA4" s="3">
         <f>capex!AA4*0.05</f>
-        <v>1</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -5298,107 +5395,107 @@
       </c>
       <c r="B5" s="3">
         <f>capex!B5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="C5" s="3">
         <f>capex!C5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="D5" s="3">
         <f>capex!D5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="E5" s="3">
         <f>capex!E5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="F5" s="3">
         <f>capex!F5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="G5" s="3">
         <f>capex!G5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="H5" s="3">
         <f>capex!H5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="I5" s="3">
         <f>capex!I5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="J5" s="3">
         <f>capex!J5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="K5" s="3">
         <f>capex!K5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="L5" s="3">
         <f>capex!L5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="M5" s="3">
         <f>capex!M5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="N5" s="3">
         <f>capex!N5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="O5" s="3">
         <f>capex!O5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="P5" s="3">
         <f>capex!P5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="Q5" s="3">
         <f>capex!Q5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="R5" s="3">
         <f>capex!R5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="S5" s="3">
         <f>capex!S5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="T5" s="3">
         <f>capex!T5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="U5" s="3">
         <f>capex!U5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="V5" s="3">
         <f>capex!V5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="W5" s="3">
         <f>capex!W5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="X5" s="3">
         <f>capex!X5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="Y5" s="3">
         <f>capex!Y5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="Z5" s="3">
         <f>capex!Z5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
       <c r="AA5" s="3">
         <f>capex!AA5*0.05</f>
-        <v>2.25</v>
+        <v>37.5</v>
       </c>
     </row>
   </sheetData>
@@ -5506,107 +5603,107 @@
       </c>
       <c r="B2" s="3">
         <f>capex!B2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="C2" s="3">
         <f>capex!C2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="D2" s="3">
         <f>capex!D2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="E2" s="3">
         <f>capex!E2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="F2" s="3">
         <f>capex!F2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="G2" s="3">
         <f>capex!G2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="H2" s="3">
         <f>capex!H2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="I2" s="3">
         <f>capex!I2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="J2" s="3">
         <f>capex!J2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="K2" s="3">
         <f>capex!K2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="L2" s="3">
         <f>capex!L2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="M2" s="3">
         <f>capex!M2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="N2" s="3">
         <f>capex!N2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="O2" s="3">
         <f>capex!O2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="P2" s="3">
         <f>capex!P2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="Q2" s="3">
         <f>capex!Q2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="R2" s="3">
         <f>capex!R2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="S2" s="3">
         <f>capex!S2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="T2" s="3">
         <f>capex!T2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="U2" s="3">
         <f>capex!U2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="V2" s="3">
         <f>capex!V2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="W2" s="3">
         <f>capex!W2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="X2" s="3">
         <f>capex!X2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="Y2" s="3">
         <f>capex!Y2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="Z2" s="3">
         <f>capex!Z2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
       <c r="AA2" s="3">
         <f>capex!AA2*0.25</f>
-        <v>7.5</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
@@ -5615,107 +5712,107 @@
       </c>
       <c r="B3" s="3">
         <f>capex!B3*0.25</f>
-        <v>37.5</v>
+        <v>2250</v>
       </c>
       <c r="C3" s="3">
         <f>capex!C3*0.25</f>
-        <v>36.333333333333329</v>
+        <v>2250</v>
       </c>
       <c r="D3" s="3">
         <f>capex!D3*0.25</f>
-        <v>35.166666666666664</v>
+        <v>2250</v>
       </c>
       <c r="E3" s="3">
         <f>capex!E3*0.25</f>
-        <v>34</v>
+        <v>2250</v>
       </c>
       <c r="F3" s="3">
         <f>capex!F3*0.25</f>
-        <v>32.833333333333336</v>
+        <v>2250</v>
       </c>
       <c r="G3" s="3">
         <f>capex!G3*0.25</f>
-        <v>31.666666666666664</v>
+        <v>2250</v>
       </c>
       <c r="H3" s="3">
         <f>capex!H3*0.25</f>
-        <v>30.5</v>
+        <v>2250</v>
       </c>
       <c r="I3" s="3">
         <f>capex!I3*0.25</f>
-        <v>29.333333333333336</v>
+        <v>2250</v>
       </c>
       <c r="J3" s="3">
         <f>capex!J3*0.25</f>
-        <v>28.166666666666668</v>
+        <v>2250</v>
       </c>
       <c r="K3" s="3">
         <f>capex!K3*0.25</f>
-        <v>27</v>
+        <v>2250</v>
       </c>
       <c r="L3" s="3">
         <f>capex!L3*0.25</f>
-        <v>25.833333333333336</v>
+        <v>75</v>
       </c>
       <c r="M3" s="3">
         <f>capex!M3*0.25</f>
-        <v>24.666666666666668</v>
+        <v>75</v>
       </c>
       <c r="N3" s="3">
         <f>capex!N3*0.25</f>
-        <v>12.5</v>
+        <v>75</v>
       </c>
       <c r="O3" s="3">
         <f>capex!O3*0.25</f>
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="P3" s="3">
         <f>capex!P3*0.25</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="3">
         <f>capex!Q3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="R3" s="3">
         <f>capex!R3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="S3" s="3">
         <f>capex!S3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="T3" s="3">
         <f>capex!T3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="U3" s="3">
         <f>capex!U3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="V3" s="3">
         <f>capex!V3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="W3" s="3">
         <f>capex!W3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="X3" s="3">
         <f>capex!X3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Y3" s="3">
         <f>capex!Y3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Z3" s="3">
         <f>capex!Z3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AA3" s="3">
         <f>capex!AA3*0.25</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
@@ -5724,107 +5821,107 @@
       </c>
       <c r="B4" s="3">
         <f>capex!B4*0.25</f>
-        <v>20</v>
+        <v>1125</v>
       </c>
       <c r="C4" s="3">
         <f>capex!C4*0.25</f>
-        <v>19.75</v>
+        <v>1125</v>
       </c>
       <c r="D4" s="3">
         <f>capex!D4*0.25</f>
-        <v>19.5</v>
+        <v>1125</v>
       </c>
       <c r="E4" s="3">
         <f>capex!E4*0.25</f>
-        <v>19.25</v>
+        <v>1125</v>
       </c>
       <c r="F4" s="3">
         <f>capex!F4*0.25</f>
-        <v>19</v>
+        <v>1125</v>
       </c>
       <c r="G4" s="3">
         <f>capex!G4*0.25</f>
-        <v>18.75</v>
+        <v>1125</v>
       </c>
       <c r="H4" s="3">
         <f>capex!H4*0.25</f>
-        <v>18.5</v>
+        <v>1125</v>
       </c>
       <c r="I4" s="3">
         <f>capex!I4*0.25</f>
-        <v>18.25</v>
+        <v>1125</v>
       </c>
       <c r="J4" s="3">
         <f>capex!J4*0.25</f>
-        <v>18</v>
+        <v>1125</v>
       </c>
       <c r="K4" s="3">
         <f>capex!K4*0.25</f>
-        <v>17.75</v>
+        <v>1125</v>
       </c>
       <c r="L4" s="3">
         <f>capex!L4*0.25</f>
-        <v>17.5</v>
+        <v>1125</v>
       </c>
       <c r="M4" s="3">
         <f>capex!M4*0.25</f>
-        <v>17.25</v>
+        <v>1125</v>
       </c>
       <c r="N4" s="3">
         <f>capex!N4*0.25</f>
-        <v>17</v>
+        <v>1125</v>
       </c>
       <c r="O4" s="3">
         <f>capex!O4*0.25</f>
-        <v>16.75</v>
+        <v>1125</v>
       </c>
       <c r="P4" s="3">
         <f>capex!P4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="Q4" s="3">
         <f>capex!Q4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="R4" s="3">
         <f>capex!R4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="S4" s="3">
         <f>capex!S4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="T4" s="3">
         <f>capex!T4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="U4" s="3">
         <f>capex!U4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="V4" s="3">
         <f>capex!V4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="W4" s="3">
         <f>capex!W4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="X4" s="3">
         <f>capex!X4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="Y4" s="3">
         <f>capex!Y4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="Z4" s="3">
         <f>capex!Z4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
       <c r="AA4" s="3">
         <f>capex!AA4*0.25</f>
-        <v>5</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -5833,107 +5930,107 @@
       </c>
       <c r="B5" s="3">
         <f>capex!B5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="C5" s="3">
         <f>capex!C5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="D5" s="3">
         <f>capex!D5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="E5" s="3">
         <f>capex!E5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="F5" s="3">
         <f>capex!F5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="G5" s="3">
         <f>capex!G5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="H5" s="3">
         <f>capex!H5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="I5" s="3">
         <f>capex!I5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="J5" s="3">
         <f>capex!J5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="K5" s="3">
         <f>capex!K5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="L5" s="3">
         <f>capex!L5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="M5" s="3">
         <f>capex!M5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="N5" s="3">
         <f>capex!N5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="O5" s="3">
         <f>capex!O5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="P5" s="3">
         <f>capex!P5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="Q5" s="3">
         <f>capex!Q5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="R5" s="3">
         <f>capex!R5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="S5" s="3">
         <f>capex!S5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="T5" s="3">
         <f>capex!T5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="U5" s="3">
         <f>capex!U5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="V5" s="3">
         <f>capex!V5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="W5" s="3">
         <f>capex!W5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="X5" s="3">
         <f>capex!X5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="Y5" s="3">
         <f>capex!Y5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="Z5" s="3">
         <f>capex!Z5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
       <c r="AA5" s="3">
         <f>capex!AA5*0.25</f>
-        <v>11.25</v>
+        <v>187.5</v>
       </c>
     </row>
   </sheetData>
@@ -5947,7 +6044,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5973,7 +6070,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>2020</v>
@@ -5984,7 +6081,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>2040</v>
@@ -5995,7 +6092,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>2020</v>
@@ -6006,7 +6103,7 @@
         <v>49</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>2030</v>

</xml_diff>

<commit_message>
Clean System Level Clean System Wide
</commit_message>
<xml_diff>
--- a/database/steel_data.xlsx
+++ b/database/steel_data.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PLANiT\github\macc_steel\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED2E909-18D3-42C5-BB5F-617C161BD252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB20CF58-D683-4D95-B1EA-AA94F2EDB4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="2064" windowWidth="23760" windowHeight="19476" tabRatio="620" firstSheet="12" activeTab="12" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
+    <workbookView xWindow="-28910" yWindow="-110" windowWidth="29020" windowHeight="17500" tabRatio="620" firstSheet="7" activeTab="12" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="18" r:id="rId1"/>
     <sheet name="baseline" sheetId="7" r:id="rId2"/>
-    <sheet name="emission_system" sheetId="24" r:id="rId3"/>
-    <sheet name="capex" sheetId="13" r:id="rId4"/>
-    <sheet name="opex" sheetId="14" r:id="rId5"/>
-    <sheet name="renewal" sheetId="15" r:id="rId6"/>
-    <sheet name="technology" sheetId="19" r:id="rId7"/>
-    <sheet name="technology_ei" sheetId="21" r:id="rId8"/>
-    <sheet name="emission" sheetId="23" r:id="rId9"/>
+    <sheet name="capex" sheetId="13" r:id="rId3"/>
+    <sheet name="opex" sheetId="14" r:id="rId4"/>
+    <sheet name="renewal" sheetId="15" r:id="rId5"/>
+    <sheet name="technology" sheetId="19" r:id="rId6"/>
+    <sheet name="technology_ei" sheetId="21" r:id="rId7"/>
+    <sheet name="emission" sheetId="23" r:id="rId8"/>
+    <sheet name="emission_system" sheetId="24" r:id="rId9"/>
     <sheet name="material_cost" sheetId="11" r:id="rId10"/>
     <sheet name="material_emission" sheetId="12" r:id="rId11"/>
     <sheet name="material_efficiency" sheetId="17" r:id="rId12"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="55">
   <si>
     <t>BF-BOF</t>
   </si>
@@ -255,6 +255,10 @@
   </si>
   <si>
     <t>global</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2169,10 +2173,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A5865B-B011-402F-A09D-739FDD6B0E90}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2180,7 +2184,7 @@
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -2190,8 +2194,11 @@
       <c r="C1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2199,10 +2206,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2210,10 +2220,13 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2221,10 +2234,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+        <v>0.4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2234,8 +2250,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2243,10 +2262,13 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2256,8 +2278,11 @@
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2265,10 +2290,13 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.4">
+        <v>0.2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -2278,8 +2306,11 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="D9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -2287,7 +2318,10 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2298,10 +2332,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A8B42D-00EB-470C-A0D2-7C21A6CB877B}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2309,7 +2343,7 @@
     <col min="3" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -2319,8 +2353,11 @@
       <c r="C1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2330,65 +2367,107 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.4">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4061,440 +4140,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E683ACB1-236C-41D9-AD28-376C61929EF9}">
-  <dimension ref="A1:AA5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1">
-        <v>2025</v>
-      </c>
-      <c r="C1">
-        <v>2026</v>
-      </c>
-      <c r="D1">
-        <v>2027</v>
-      </c>
-      <c r="E1">
-        <v>2028</v>
-      </c>
-      <c r="F1">
-        <v>2029</v>
-      </c>
-      <c r="G1">
-        <v>2030</v>
-      </c>
-      <c r="H1">
-        <v>2031</v>
-      </c>
-      <c r="I1">
-        <v>2032</v>
-      </c>
-      <c r="J1">
-        <v>2033</v>
-      </c>
-      <c r="K1">
-        <v>2034</v>
-      </c>
-      <c r="L1">
-        <v>2035</v>
-      </c>
-      <c r="M1">
-        <v>2036</v>
-      </c>
-      <c r="N1">
-        <v>2037</v>
-      </c>
-      <c r="O1">
-        <v>2038</v>
-      </c>
-      <c r="P1">
-        <v>2039</v>
-      </c>
-      <c r="Q1">
-        <v>2040</v>
-      </c>
-      <c r="R1">
-        <v>2041</v>
-      </c>
-      <c r="S1">
-        <v>2042</v>
-      </c>
-      <c r="T1">
-        <v>2043</v>
-      </c>
-      <c r="U1">
-        <v>2044</v>
-      </c>
-      <c r="V1">
-        <v>2045</v>
-      </c>
-      <c r="W1">
-        <v>2046</v>
-      </c>
-      <c r="X1">
-        <v>2047</v>
-      </c>
-      <c r="Y1">
-        <v>2048</v>
-      </c>
-      <c r="Z1">
-        <v>2049</v>
-      </c>
-      <c r="AA1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>99999999</v>
-      </c>
-      <c r="C2">
-        <v>1000000</v>
-      </c>
-      <c r="D2">
-        <v>1000000</v>
-      </c>
-      <c r="E2">
-        <v>1000000</v>
-      </c>
-      <c r="F2">
-        <v>1000000</v>
-      </c>
-      <c r="G2">
-        <v>1000000</v>
-      </c>
-      <c r="H2">
-        <v>1000000</v>
-      </c>
-      <c r="I2">
-        <v>1000000</v>
-      </c>
-      <c r="J2">
-        <v>1000000</v>
-      </c>
-      <c r="K2">
-        <v>1000000</v>
-      </c>
-      <c r="L2">
-        <v>1000000</v>
-      </c>
-      <c r="M2">
-        <v>1000000</v>
-      </c>
-      <c r="N2">
-        <v>1000000</v>
-      </c>
-      <c r="O2">
-        <v>1000000</v>
-      </c>
-      <c r="P2">
-        <v>1000000</v>
-      </c>
-      <c r="Q2">
-        <v>1000000</v>
-      </c>
-      <c r="R2">
-        <v>1000000</v>
-      </c>
-      <c r="S2">
-        <v>1000000</v>
-      </c>
-      <c r="T2">
-        <v>1000000</v>
-      </c>
-      <c r="U2">
-        <v>1000000</v>
-      </c>
-      <c r="V2">
-        <v>1000000</v>
-      </c>
-      <c r="W2">
-        <v>1000000</v>
-      </c>
-      <c r="X2">
-        <v>1000000</v>
-      </c>
-      <c r="Y2">
-        <v>1000000</v>
-      </c>
-      <c r="Z2">
-        <v>1000000</v>
-      </c>
-      <c r="AA2">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>99999999</v>
-      </c>
-      <c r="C3">
-        <v>1000000</v>
-      </c>
-      <c r="D3">
-        <v>1000000</v>
-      </c>
-      <c r="E3">
-        <v>1000000</v>
-      </c>
-      <c r="F3">
-        <v>1000000</v>
-      </c>
-      <c r="G3">
-        <v>1000000</v>
-      </c>
-      <c r="H3">
-        <v>1000000</v>
-      </c>
-      <c r="I3">
-        <v>1000000</v>
-      </c>
-      <c r="J3">
-        <v>1000000</v>
-      </c>
-      <c r="K3">
-        <v>1000000</v>
-      </c>
-      <c r="L3">
-        <v>1000000</v>
-      </c>
-      <c r="M3">
-        <v>1000000</v>
-      </c>
-      <c r="N3">
-        <v>1000000</v>
-      </c>
-      <c r="O3">
-        <v>1000000</v>
-      </c>
-      <c r="P3">
-        <v>1000000</v>
-      </c>
-      <c r="Q3">
-        <v>1000000</v>
-      </c>
-      <c r="R3">
-        <v>1000000</v>
-      </c>
-      <c r="S3">
-        <v>1000000</v>
-      </c>
-      <c r="T3">
-        <v>1000000</v>
-      </c>
-      <c r="U3">
-        <v>1000000</v>
-      </c>
-      <c r="V3">
-        <v>1000000</v>
-      </c>
-      <c r="W3">
-        <v>1000000</v>
-      </c>
-      <c r="X3">
-        <v>1000000</v>
-      </c>
-      <c r="Y3">
-        <v>1000000</v>
-      </c>
-      <c r="Z3">
-        <v>1000000</v>
-      </c>
-      <c r="AA3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>99999999</v>
-      </c>
-      <c r="C4">
-        <v>100000</v>
-      </c>
-      <c r="D4">
-        <v>100000</v>
-      </c>
-      <c r="E4">
-        <v>100000</v>
-      </c>
-      <c r="F4">
-        <v>100000</v>
-      </c>
-      <c r="G4">
-        <v>100000</v>
-      </c>
-      <c r="H4">
-        <v>100000</v>
-      </c>
-      <c r="I4">
-        <v>100000</v>
-      </c>
-      <c r="J4">
-        <v>100000</v>
-      </c>
-      <c r="K4">
-        <v>100000</v>
-      </c>
-      <c r="L4">
-        <v>100000</v>
-      </c>
-      <c r="M4">
-        <v>100000</v>
-      </c>
-      <c r="N4">
-        <v>100000</v>
-      </c>
-      <c r="O4">
-        <v>100000</v>
-      </c>
-      <c r="P4">
-        <v>100000</v>
-      </c>
-      <c r="Q4">
-        <v>100000</v>
-      </c>
-      <c r="R4">
-        <v>100000</v>
-      </c>
-      <c r="S4">
-        <v>100000</v>
-      </c>
-      <c r="T4">
-        <v>100000</v>
-      </c>
-      <c r="U4">
-        <v>100000</v>
-      </c>
-      <c r="V4">
-        <v>100000</v>
-      </c>
-      <c r="W4">
-        <v>100000</v>
-      </c>
-      <c r="X4">
-        <v>100000</v>
-      </c>
-      <c r="Y4">
-        <v>100000</v>
-      </c>
-      <c r="Z4">
-        <v>100000</v>
-      </c>
-      <c r="AA4">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>99999999</v>
-      </c>
-      <c r="C5">
-        <v>100000</v>
-      </c>
-      <c r="D5">
-        <v>100000</v>
-      </c>
-      <c r="E5">
-        <v>100000</v>
-      </c>
-      <c r="F5">
-        <v>100000</v>
-      </c>
-      <c r="G5">
-        <v>100000</v>
-      </c>
-      <c r="H5">
-        <v>100000</v>
-      </c>
-      <c r="I5">
-        <v>100000</v>
-      </c>
-      <c r="J5">
-        <v>100000</v>
-      </c>
-      <c r="K5">
-        <v>100000</v>
-      </c>
-      <c r="L5">
-        <v>100000</v>
-      </c>
-      <c r="M5">
-        <v>100000</v>
-      </c>
-      <c r="N5">
-        <v>100000</v>
-      </c>
-      <c r="O5">
-        <v>100000</v>
-      </c>
-      <c r="P5">
-        <v>100000</v>
-      </c>
-      <c r="Q5">
-        <v>100000</v>
-      </c>
-      <c r="R5">
-        <v>100000</v>
-      </c>
-      <c r="S5">
-        <v>100000</v>
-      </c>
-      <c r="T5">
-        <v>100000</v>
-      </c>
-      <c r="U5">
-        <v>100000</v>
-      </c>
-      <c r="V5">
-        <v>100000</v>
-      </c>
-      <c r="W5">
-        <v>100000</v>
-      </c>
-      <c r="X5">
-        <v>100000</v>
-      </c>
-      <c r="Y5">
-        <v>100000</v>
-      </c>
-      <c r="Z5">
-        <v>100000</v>
-      </c>
-      <c r="AA5">
-        <v>100000</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E234AF8D-964B-419F-969D-C9FD34B2C8AE}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -4951,7 +4596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39EC2A4D-93DC-4E45-8627-2A75EDF5181B}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -5486,7 +5131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18CEE6-4CB2-4E28-86E1-E84E657A73A8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -6021,7 +5666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5339A0-3D98-43CE-86F7-53EF60721306}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -6097,7 +5742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F464A74C-C8AE-4B5D-B335-B05DB5565181}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -6528,17 +6173,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E46CCB1-2754-42FA-B5C9-8DABA83A320C}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:AA2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6630,101 +6275,556 @@
         <v>53</v>
       </c>
       <c r="B2">
+        <v>999999999</v>
+      </c>
+      <c r="C2">
+        <v>999999999</v>
+      </c>
+      <c r="D2">
+        <v>999999999</v>
+      </c>
+      <c r="E2">
+        <v>999999999</v>
+      </c>
+      <c r="F2">
+        <v>999999999</v>
+      </c>
+      <c r="G2">
+        <v>999999999</v>
+      </c>
+      <c r="H2">
+        <v>999999999</v>
+      </c>
+      <c r="I2">
+        <v>999999999</v>
+      </c>
+      <c r="J2">
+        <v>999999999</v>
+      </c>
+      <c r="K2">
+        <v>999999999</v>
+      </c>
+      <c r="L2">
+        <v>999999999</v>
+      </c>
+      <c r="M2">
+        <v>999999999</v>
+      </c>
+      <c r="N2">
+        <v>999999999</v>
+      </c>
+      <c r="O2">
+        <v>999999999</v>
+      </c>
+      <c r="P2">
+        <v>999999999</v>
+      </c>
+      <c r="Q2">
+        <v>999999999</v>
+      </c>
+      <c r="R2">
+        <v>999999999</v>
+      </c>
+      <c r="S2">
+        <v>999999999</v>
+      </c>
+      <c r="T2">
+        <v>999999999</v>
+      </c>
+      <c r="U2">
+        <v>999999999</v>
+      </c>
+      <c r="V2">
+        <v>999999999</v>
+      </c>
+      <c r="W2">
+        <v>999999999</v>
+      </c>
+      <c r="X2">
+        <v>999999999</v>
+      </c>
+      <c r="Y2">
+        <v>999999999</v>
+      </c>
+      <c r="Z2">
+        <v>999999999</v>
+      </c>
+      <c r="AA2">
+        <v>999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E683ACB1-236C-41D9-AD28-376C61929EF9}">
+  <dimension ref="A1:AA5"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:AA5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>2025</v>
+      </c>
+      <c r="C1">
+        <v>2026</v>
+      </c>
+      <c r="D1">
+        <v>2027</v>
+      </c>
+      <c r="E1">
+        <v>2028</v>
+      </c>
+      <c r="F1">
+        <v>2029</v>
+      </c>
+      <c r="G1">
+        <v>2030</v>
+      </c>
+      <c r="H1">
+        <v>2031</v>
+      </c>
+      <c r="I1">
+        <v>2032</v>
+      </c>
+      <c r="J1">
+        <v>2033</v>
+      </c>
+      <c r="K1">
+        <v>2034</v>
+      </c>
+      <c r="L1">
+        <v>2035</v>
+      </c>
+      <c r="M1">
+        <v>2036</v>
+      </c>
+      <c r="N1">
+        <v>2037</v>
+      </c>
+      <c r="O1">
+        <v>2038</v>
+      </c>
+      <c r="P1">
+        <v>2039</v>
+      </c>
+      <c r="Q1">
+        <v>2040</v>
+      </c>
+      <c r="R1">
+        <v>2041</v>
+      </c>
+      <c r="S1">
+        <v>2042</v>
+      </c>
+      <c r="T1">
+        <v>2043</v>
+      </c>
+      <c r="U1">
+        <v>2044</v>
+      </c>
+      <c r="V1">
+        <v>2045</v>
+      </c>
+      <c r="W1">
+        <v>2046</v>
+      </c>
+      <c r="X1">
+        <v>2047</v>
+      </c>
+      <c r="Y1">
+        <v>2048</v>
+      </c>
+      <c r="Z1">
+        <v>2049</v>
+      </c>
+      <c r="AA1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>99999999</v>
+      </c>
+      <c r="C2">
         <v>10000000</v>
       </c>
-      <c r="C2">
-        <f>B2*0.5</f>
+      <c r="D2">
+        <v>10000000</v>
+      </c>
+      <c r="E2">
+        <v>10000000</v>
+      </c>
+      <c r="F2">
+        <v>10000000</v>
+      </c>
+      <c r="G2">
+        <v>10000000</v>
+      </c>
+      <c r="H2">
+        <f>G2/2</f>
         <v>5000000</v>
       </c>
-      <c r="D2">
-        <f>C2</f>
-        <v>5000000</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:F2" si="0">D2</f>
-        <v>5000000</v>
-      </c>
-      <c r="F2">
-        <f t="shared" si="0"/>
-        <v>5000000</v>
-      </c>
-      <c r="G2">
-        <f>F2*0.5</f>
+      <c r="I2">
+        <f t="shared" ref="I2:AA3" si="0">H2/2</f>
         <v>2500000</v>
       </c>
-      <c r="H2">
-        <f>G2</f>
+      <c r="J2">
+        <f>I2</f>
         <v>2500000</v>
       </c>
-      <c r="I2">
-        <f t="shared" ref="I2:K2" si="1">H2</f>
+      <c r="K2">
+        <f t="shared" ref="K2:AA3" si="1">J2</f>
         <v>2500000</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <f t="shared" si="1"/>
         <v>2500000</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <f t="shared" si="1"/>
         <v>2500000</v>
       </c>
-      <c r="L2">
-        <f>K2*0.5</f>
-        <v>1250000</v>
-      </c>
-      <c r="M2">
-        <f>L2</f>
-        <v>1250000</v>
-      </c>
       <c r="N2">
-        <f t="shared" ref="N2:U2" si="2">M2</f>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="O2">
-        <f t="shared" si="2"/>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="P2">
-        <f t="shared" si="2"/>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="Q2">
-        <f t="shared" si="2"/>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="R2">
-        <f t="shared" si="2"/>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="S2">
-        <f t="shared" si="2"/>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="T2">
-        <f t="shared" si="2"/>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="U2">
-        <f t="shared" si="2"/>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>99999999</v>
+      </c>
+      <c r="C3">
+        <v>10000000</v>
+      </c>
+      <c r="D3">
+        <v>10000000</v>
+      </c>
+      <c r="E3">
+        <v>10000000</v>
+      </c>
+      <c r="F3">
+        <v>10000000</v>
+      </c>
+      <c r="G3">
+        <v>10000000</v>
+      </c>
+      <c r="H3">
+        <f>G3/2</f>
+        <v>5000000</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>2500000</v>
+      </c>
+      <c r="J3">
+        <f>I3</f>
+        <v>2500000</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="X3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" si="1"/>
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>99999999</v>
+      </c>
+      <c r="C4">
+        <v>10000000</v>
+      </c>
+      <c r="D4">
+        <v>10000000</v>
+      </c>
+      <c r="E4">
+        <v>10000000</v>
+      </c>
+      <c r="F4">
+        <v>10000000</v>
+      </c>
+      <c r="G4">
+        <v>10000000</v>
+      </c>
+      <c r="H4">
+        <v>500000</v>
+      </c>
+      <c r="I4">
+        <v>500000</v>
+      </c>
+      <c r="J4">
+        <v>500000</v>
+      </c>
+      <c r="K4">
+        <v>500000</v>
+      </c>
+      <c r="L4">
+        <v>500000</v>
+      </c>
+      <c r="M4">
+        <v>500000</v>
+      </c>
+      <c r="N4">
+        <v>500000</v>
+      </c>
+      <c r="O4">
+        <v>500000</v>
+      </c>
+      <c r="P4">
+        <v>500000</v>
+      </c>
+      <c r="Q4">
+        <v>500000</v>
+      </c>
+      <c r="R4">
+        <v>500000</v>
+      </c>
+      <c r="S4">
+        <v>500000</v>
+      </c>
+      <c r="T4">
+        <v>500000</v>
+      </c>
+      <c r="U4">
+        <v>500000</v>
+      </c>
+      <c r="V4">
+        <v>500000</v>
+      </c>
+      <c r="W4">
+        <v>500000</v>
+      </c>
+      <c r="X4">
+        <v>500000</v>
+      </c>
+      <c r="Y4">
+        <v>500000</v>
+      </c>
+      <c r="Z4">
+        <v>500000</v>
+      </c>
+      <c r="AA4">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>99999999</v>
+      </c>
+      <c r="C5">
+        <v>10000000</v>
+      </c>
+      <c r="D5">
+        <v>10000000</v>
+      </c>
+      <c r="E5">
+        <v>10000000</v>
+      </c>
+      <c r="F5">
+        <v>10000000</v>
+      </c>
+      <c r="G5">
+        <v>10000000</v>
+      </c>
+      <c r="H5">
+        <v>500000</v>
+      </c>
+      <c r="I5">
+        <v>500000</v>
+      </c>
+      <c r="J5">
+        <v>500000</v>
+      </c>
+      <c r="K5">
+        <v>500000</v>
+      </c>
+      <c r="L5">
+        <v>500000</v>
+      </c>
+      <c r="M5">
+        <v>500000</v>
+      </c>
+      <c r="N5">
+        <v>500000</v>
+      </c>
+      <c r="O5">
+        <v>500000</v>
+      </c>
+      <c r="P5">
+        <v>500000</v>
+      </c>
+      <c r="Q5">
+        <v>500000</v>
+      </c>
+      <c r="R5">
+        <v>500000</v>
+      </c>
+      <c r="S5">
+        <v>500000</v>
+      </c>
+      <c r="T5">
+        <v>500000</v>
+      </c>
+      <c r="U5">
+        <v>500000</v>
+      </c>
+      <c r="V5">
+        <v>500000</v>
+      </c>
+      <c r="W5">
+        <v>500000</v>
+      </c>
+      <c r="X5">
+        <v>500000</v>
+      </c>
+      <c r="Y5">
+        <v>500000</v>
+      </c>
+      <c r="Z5">
+        <v>500000</v>
+      </c>
+      <c r="AA5">
+        <v>500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.0 Multifuel and Introduction Years of Fuels/Materials
</commit_message>
<xml_diff>
--- a/database/steel_data.xlsx
+++ b/database/steel_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PLANiT\github\macc_steel\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C14CEC9-9F6D-41D6-BCB4-BB1D3AD2E3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9109A8-2648-47F8-AD06-E0FACA76FD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3276" yWindow="708" windowWidth="39132" windowHeight="17376" tabRatio="620" activeTab="5" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
+    <workbookView xWindow="1230" yWindow="1050" windowWidth="25690" windowHeight="15010" tabRatio="775" firstSheet="8" activeTab="14" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="18" r:id="rId1"/>
@@ -27,10 +27,12 @@
     <sheet name="material_emission" sheetId="12" r:id="rId12"/>
     <sheet name="material_efficiency" sheetId="17" r:id="rId13"/>
     <sheet name="technology_fuel_pairs" sheetId="5" r:id="rId14"/>
-    <sheet name="technology_material_pairs" sheetId="6" r:id="rId15"/>
-    <sheet name="fuel_cost" sheetId="8" r:id="rId16"/>
-    <sheet name="fuel_efficiency" sheetId="16" r:id="rId17"/>
-    <sheet name="fuel_emission" sheetId="10" r:id="rId18"/>
+    <sheet name="fuel_introduction" sheetId="26" r:id="rId15"/>
+    <sheet name="material_introduction" sheetId="27" r:id="rId16"/>
+    <sheet name="technology_material_pairs" sheetId="6" r:id="rId17"/>
+    <sheet name="fuel_cost" sheetId="8" r:id="rId18"/>
+    <sheet name="fuel_efficiency" sheetId="16" r:id="rId19"/>
+    <sheet name="fuel_emission" sheetId="10" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="66">
   <si>
     <t>BF-BOF</t>
   </si>
@@ -268,6 +270,42 @@
   </si>
   <si>
     <t>currency / ton-CO2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>currency / ton-capacity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>levelised</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>per capacity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>note</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuel_share</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>material_share</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8, 0.2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cokes, Scrap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NG-DRI</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -679,51 +717,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21BDFBF-8BC3-41DF-97CA-33C5F9721F61}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -731,15 +782,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -747,7 +801,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -755,23 +809,29 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -779,7 +839,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -787,7 +847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -806,15 +866,15 @@
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B2" sqref="B2:AA5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -897,7 +957,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -905,102 +965,82 @@
         <v>99999999</v>
       </c>
       <c r="C2">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="D2">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="E2">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="F2">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="G2">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="H2">
-        <f>G2/2</f>
-        <v>5000000</v>
+        <v>99999999</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I3" si="0">H2/2</f>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="J2">
-        <f>I2</f>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:AA3" si="1">J2</f>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="L2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="M2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="N2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="O2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="P2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="Q2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="R2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="S2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="T2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="U2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="V2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="W2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="X2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="Y2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="Z2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="AA2">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1008,102 +1048,82 @@
         <v>99999999</v>
       </c>
       <c r="C3">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="D3">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="E3">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="F3">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="G3">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="H3">
-        <f>G3/2</f>
-        <v>5000000</v>
+        <v>99999999</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="J3">
-        <f>I3</f>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="K3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="L3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="M3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="N3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="O3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="P3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="R3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="S3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="T3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="U3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="V3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="W3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="X3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
+        <v>99999999</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1111,82 +1131,82 @@
         <v>99999999</v>
       </c>
       <c r="C4">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="D4">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="E4">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="F4">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="G4">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="H4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="I4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="J4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="K4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="L4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="M4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="N4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="O4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="P4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="Q4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="R4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="S4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="T4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="U4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="V4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="W4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="X4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="Y4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="Z4">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="AA4">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1194,79 +1214,79 @@
         <v>99999999</v>
       </c>
       <c r="C5">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="D5">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="E5">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="F5">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="G5">
-        <v>10000000</v>
+        <v>99999999</v>
       </c>
       <c r="H5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="I5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="J5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="K5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="L5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="M5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="N5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="O5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="P5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="Q5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="R5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="S5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="T5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="U5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="V5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="W5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="X5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="Y5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="Z5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
       <c r="AA5">
-        <v>500000</v>
+        <v>99999999</v>
       </c>
     </row>
   </sheetData>
@@ -1280,15 +1300,15 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="27" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="27" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -1371,7 +1391,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1454,7 +1474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1537,7 +1557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1620,7 +1640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1703,7 +1723,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1743,16 +1763,16 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="R43" sqref="R43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="27" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="27" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -1835,7 +1855,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1918,7 +1938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2001,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2084,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2167,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2210,9 +2230,9 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -2295,7 +2315,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2378,7 +2398,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2461,7 +2481,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2544,7 +2564,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2627,7 +2647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2664,18 +2684,18 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A5865B-B011-402F-A09D-739FDD6B0E90}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -2688,8 +2708,11 @@
       <c r="D1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2702,8 +2725,11 @@
       <c r="D2">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2714,10 +2740,13 @@
         <v>0.5</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2730,8 +2759,11 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2744,8 +2776,11 @@
       <c r="D5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E5">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2753,13 +2788,16 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2772,8 +2810,11 @@
       <c r="D7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2786,8 +2827,11 @@
       <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -2800,8 +2844,11 @@
       <c r="D9">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -2813,6 +2860,9 @@
       </c>
       <c r="D10">
         <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -2822,142 +2872,61 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A8B42D-00EB-470C-A0D2-7C21A6CB877B}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A811D9-2602-4FD1-8BF7-F55E2D4AA43D}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="3" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3">
-        <v>0.5</v>
-      </c>
-      <c r="D3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>0.2</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>0.2</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2035</v>
       </c>
     </row>
   </sheetData>
@@ -2967,511 +2936,53 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251D8908-2320-4E41-AC8F-86BD7BF58C9B}">
-  <dimension ref="A1:AA6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{410A1906-5A3B-4FF2-8752-8FE09D0C1871}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:AA6"/>
+      <selection activeCell="B4" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1">
-        <v>2025</v>
-      </c>
-      <c r="C1">
-        <v>2026</v>
-      </c>
-      <c r="D1">
-        <v>2027</v>
-      </c>
-      <c r="E1">
-        <v>2028</v>
-      </c>
-      <c r="F1">
-        <v>2029</v>
-      </c>
-      <c r="G1">
-        <v>2030</v>
-      </c>
-      <c r="H1">
-        <v>2031</v>
-      </c>
-      <c r="I1">
-        <v>2032</v>
-      </c>
-      <c r="J1">
-        <v>2033</v>
-      </c>
-      <c r="K1">
-        <v>2034</v>
-      </c>
-      <c r="L1">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
         <v>2035</v>
       </c>
-      <c r="M1">
-        <v>2036</v>
-      </c>
-      <c r="N1">
-        <v>2037</v>
-      </c>
-      <c r="O1">
-        <v>2038</v>
-      </c>
-      <c r="P1">
-        <v>2039</v>
-      </c>
-      <c r="Q1">
-        <v>2040</v>
-      </c>
-      <c r="R1">
-        <v>2041</v>
-      </c>
-      <c r="S1">
-        <v>2042</v>
-      </c>
-      <c r="T1">
-        <v>2043</v>
-      </c>
-      <c r="U1">
-        <v>2044</v>
-      </c>
-      <c r="V1">
-        <v>2045</v>
-      </c>
-      <c r="W1">
-        <v>2046</v>
-      </c>
-      <c r="X1">
-        <v>2047</v>
-      </c>
-      <c r="Y1">
-        <v>2048</v>
-      </c>
-      <c r="Z1">
-        <v>2049</v>
-      </c>
-      <c r="AA1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5">
-        <v>5</v>
-      </c>
-      <c r="G2" s="5">
-        <v>5</v>
-      </c>
-      <c r="H2" s="5">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5">
-        <v>5</v>
-      </c>
-      <c r="J2" s="5">
-        <v>5</v>
-      </c>
-      <c r="K2" s="5">
-        <v>5</v>
-      </c>
-      <c r="L2" s="5">
-        <v>5</v>
-      </c>
-      <c r="M2" s="5">
-        <v>5</v>
-      </c>
-      <c r="N2" s="5">
-        <v>5</v>
-      </c>
-      <c r="O2" s="5">
-        <v>5</v>
-      </c>
-      <c r="P2" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>5</v>
-      </c>
-      <c r="R2" s="5">
-        <v>5</v>
-      </c>
-      <c r="S2" s="5">
-        <v>5</v>
-      </c>
-      <c r="T2" s="5">
-        <v>5</v>
-      </c>
-      <c r="U2" s="5">
-        <v>5</v>
-      </c>
-      <c r="V2" s="5">
-        <v>5</v>
-      </c>
-      <c r="W2" s="5">
-        <v>5</v>
-      </c>
-      <c r="X2" s="5">
-        <v>5</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>5</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>5</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>2</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5">
-        <v>2</v>
-      </c>
-      <c r="H3" s="5">
-        <v>2</v>
-      </c>
-      <c r="I3" s="5">
-        <v>2</v>
-      </c>
-      <c r="J3" s="5">
-        <v>2</v>
-      </c>
-      <c r="K3" s="5">
-        <v>2</v>
-      </c>
-      <c r="L3" s="5">
-        <v>2</v>
-      </c>
-      <c r="M3" s="5">
-        <v>2</v>
-      </c>
-      <c r="N3" s="5">
-        <v>2</v>
-      </c>
-      <c r="O3" s="5">
-        <v>2</v>
-      </c>
-      <c r="P3" s="5">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>2</v>
-      </c>
-      <c r="R3" s="5">
-        <v>2</v>
-      </c>
-      <c r="S3" s="5">
-        <v>2</v>
-      </c>
-      <c r="T3" s="5">
-        <v>2</v>
-      </c>
-      <c r="U3" s="5">
-        <v>2</v>
-      </c>
-      <c r="V3" s="5">
-        <v>2</v>
-      </c>
-      <c r="W3" s="5">
-        <v>2</v>
-      </c>
-      <c r="X3" s="5">
-        <v>2</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>2</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="J4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="M4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="N4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="O4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="P4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="R4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="S4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="T4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="U4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="V4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="W4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="X4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="Y4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="Z4" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="AA4" s="5">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5">
-        <v>5</v>
-      </c>
-      <c r="F5" s="5">
-        <v>5</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="O5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="P5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="R5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="S5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="T5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="U5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="V5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="W5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="X5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="Y5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="Z5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0</v>
-      </c>
-      <c r="M6" s="5">
-        <v>0</v>
-      </c>
-      <c r="N6" s="5">
-        <v>0</v>
-      </c>
-      <c r="O6" s="5">
-        <v>0</v>
-      </c>
-      <c r="P6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>0</v>
-      </c>
-      <c r="R6" s="5">
-        <v>0</v>
-      </c>
-      <c r="S6" s="5">
-        <v>0</v>
-      </c>
-      <c r="T6" s="5">
-        <v>0</v>
-      </c>
-      <c r="U6" s="5">
-        <v>0</v>
-      </c>
-      <c r="V6" s="5">
-        <v>0</v>
-      </c>
-      <c r="W6" s="5">
-        <v>0</v>
-      </c>
-      <c r="X6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="5">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -3481,6 +2992,709 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A8B42D-00EB-470C-A0D2-7C21A6CB877B}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="9.4140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+      <c r="E2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.8</v>
+      </c>
+      <c r="E9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251D8908-2320-4E41-AC8F-86BD7BF58C9B}">
+  <dimension ref="A1:AA6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1">
+        <v>2025</v>
+      </c>
+      <c r="C1">
+        <v>2026</v>
+      </c>
+      <c r="D1">
+        <v>2027</v>
+      </c>
+      <c r="E1">
+        <v>2028</v>
+      </c>
+      <c r="F1">
+        <v>2029</v>
+      </c>
+      <c r="G1">
+        <v>2030</v>
+      </c>
+      <c r="H1">
+        <v>2031</v>
+      </c>
+      <c r="I1">
+        <v>2032</v>
+      </c>
+      <c r="J1">
+        <v>2033</v>
+      </c>
+      <c r="K1">
+        <v>2034</v>
+      </c>
+      <c r="L1">
+        <v>2035</v>
+      </c>
+      <c r="M1">
+        <v>2036</v>
+      </c>
+      <c r="N1">
+        <v>2037</v>
+      </c>
+      <c r="O1">
+        <v>2038</v>
+      </c>
+      <c r="P1">
+        <v>2039</v>
+      </c>
+      <c r="Q1">
+        <v>2040</v>
+      </c>
+      <c r="R1">
+        <v>2041</v>
+      </c>
+      <c r="S1">
+        <v>2042</v>
+      </c>
+      <c r="T1">
+        <v>2043</v>
+      </c>
+      <c r="U1">
+        <v>2044</v>
+      </c>
+      <c r="V1">
+        <v>2045</v>
+      </c>
+      <c r="W1">
+        <v>2046</v>
+      </c>
+      <c r="X1">
+        <v>2047</v>
+      </c>
+      <c r="Y1">
+        <v>2048</v>
+      </c>
+      <c r="Z1">
+        <v>2049</v>
+      </c>
+      <c r="AA1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5">
+        <v>5</v>
+      </c>
+      <c r="J2" s="5">
+        <v>5</v>
+      </c>
+      <c r="K2" s="5">
+        <v>5</v>
+      </c>
+      <c r="L2" s="5">
+        <v>5</v>
+      </c>
+      <c r="M2" s="5">
+        <v>5</v>
+      </c>
+      <c r="N2" s="5">
+        <v>5</v>
+      </c>
+      <c r="O2" s="5">
+        <v>5</v>
+      </c>
+      <c r="P2" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>5</v>
+      </c>
+      <c r="R2" s="5">
+        <v>5</v>
+      </c>
+      <c r="S2" s="5">
+        <v>5</v>
+      </c>
+      <c r="T2" s="5">
+        <v>5</v>
+      </c>
+      <c r="U2" s="5">
+        <v>5</v>
+      </c>
+      <c r="V2" s="5">
+        <v>5</v>
+      </c>
+      <c r="W2" s="5">
+        <v>5</v>
+      </c>
+      <c r="X2" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5">
+        <v>2</v>
+      </c>
+      <c r="K3" s="5">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5">
+        <v>2</v>
+      </c>
+      <c r="M3" s="5">
+        <v>2</v>
+      </c>
+      <c r="N3" s="5">
+        <v>2</v>
+      </c>
+      <c r="O3" s="5">
+        <v>2</v>
+      </c>
+      <c r="P3" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>2</v>
+      </c>
+      <c r="R3" s="5">
+        <v>2</v>
+      </c>
+      <c r="S3" s="5">
+        <v>2</v>
+      </c>
+      <c r="T3" s="5">
+        <v>2</v>
+      </c>
+      <c r="U3" s="5">
+        <v>2</v>
+      </c>
+      <c r="V3" s="5">
+        <v>2</v>
+      </c>
+      <c r="W3" s="5">
+        <v>2</v>
+      </c>
+      <c r="X3" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="R4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="S4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="T4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="U4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="V4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="W4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="X4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="S5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="T5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="U5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="V5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="W5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="X5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0</v>
+      </c>
+      <c r="V6" s="5">
+        <v>0</v>
+      </c>
+      <c r="W6" s="5">
+        <v>0</v>
+      </c>
+      <c r="X6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC1A385-697C-4C01-B126-79A22BD0CC72}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
@@ -3488,9 +3702,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -3573,7 +3787,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3656,7 +3870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3739,7 +3953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3822,7 +4036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -3905,7 +4119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -3986,520 +4200,6 @@
       </c>
       <c r="AA6" s="5">
         <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EB8FDB-F47B-40C2-8266-6700BCAB2D8C}">
-  <dimension ref="A1:AA6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1">
-        <v>2025</v>
-      </c>
-      <c r="C1">
-        <v>2026</v>
-      </c>
-      <c r="D1">
-        <v>2027</v>
-      </c>
-      <c r="E1">
-        <v>2028</v>
-      </c>
-      <c r="F1">
-        <v>2029</v>
-      </c>
-      <c r="G1">
-        <v>2030</v>
-      </c>
-      <c r="H1">
-        <v>2031</v>
-      </c>
-      <c r="I1">
-        <v>2032</v>
-      </c>
-      <c r="J1">
-        <v>2033</v>
-      </c>
-      <c r="K1">
-        <v>2034</v>
-      </c>
-      <c r="L1">
-        <v>2035</v>
-      </c>
-      <c r="M1">
-        <v>2036</v>
-      </c>
-      <c r="N1">
-        <v>2037</v>
-      </c>
-      <c r="O1">
-        <v>2038</v>
-      </c>
-      <c r="P1">
-        <v>2039</v>
-      </c>
-      <c r="Q1">
-        <v>2040</v>
-      </c>
-      <c r="R1">
-        <v>2041</v>
-      </c>
-      <c r="S1">
-        <v>2042</v>
-      </c>
-      <c r="T1">
-        <v>2043</v>
-      </c>
-      <c r="U1">
-        <v>2044</v>
-      </c>
-      <c r="V1">
-        <v>2045</v>
-      </c>
-      <c r="W1">
-        <v>2046</v>
-      </c>
-      <c r="X1">
-        <v>2047</v>
-      </c>
-      <c r="Y1">
-        <v>2048</v>
-      </c>
-      <c r="Z1">
-        <v>2049</v>
-      </c>
-      <c r="AA1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5">
-        <v>15</v>
-      </c>
-      <c r="D2" s="5">
-        <v>15</v>
-      </c>
-      <c r="E2" s="5">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5">
-        <v>15</v>
-      </c>
-      <c r="G2" s="5">
-        <v>15</v>
-      </c>
-      <c r="H2" s="5">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5">
-        <v>15</v>
-      </c>
-      <c r="J2" s="5">
-        <v>15</v>
-      </c>
-      <c r="K2" s="5">
-        <v>15</v>
-      </c>
-      <c r="L2" s="5">
-        <v>15</v>
-      </c>
-      <c r="M2" s="5">
-        <v>15</v>
-      </c>
-      <c r="N2" s="5">
-        <v>15</v>
-      </c>
-      <c r="O2" s="5">
-        <v>15</v>
-      </c>
-      <c r="P2" s="5">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>15</v>
-      </c>
-      <c r="R2" s="5">
-        <v>15</v>
-      </c>
-      <c r="S2" s="5">
-        <v>15</v>
-      </c>
-      <c r="T2" s="5">
-        <v>15</v>
-      </c>
-      <c r="U2" s="5">
-        <v>15</v>
-      </c>
-      <c r="V2" s="5">
-        <v>15</v>
-      </c>
-      <c r="W2" s="5">
-        <v>15</v>
-      </c>
-      <c r="X2" s="5">
-        <v>15</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>15</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5">
-        <v>7</v>
-      </c>
-      <c r="E3" s="5">
-        <v>7</v>
-      </c>
-      <c r="F3" s="5">
-        <v>7</v>
-      </c>
-      <c r="G3" s="5">
-        <v>7</v>
-      </c>
-      <c r="H3" s="5">
-        <v>7</v>
-      </c>
-      <c r="I3" s="5">
-        <v>7</v>
-      </c>
-      <c r="J3" s="5">
-        <v>7</v>
-      </c>
-      <c r="K3" s="5">
-        <v>7</v>
-      </c>
-      <c r="L3" s="5">
-        <v>7</v>
-      </c>
-      <c r="M3" s="5">
-        <v>7</v>
-      </c>
-      <c r="N3" s="5">
-        <v>7</v>
-      </c>
-      <c r="O3" s="5">
-        <v>7</v>
-      </c>
-      <c r="P3" s="5">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>7</v>
-      </c>
-      <c r="R3" s="5">
-        <v>7</v>
-      </c>
-      <c r="S3" s="5">
-        <v>7</v>
-      </c>
-      <c r="T3" s="5">
-        <v>7</v>
-      </c>
-      <c r="U3" s="5">
-        <v>7</v>
-      </c>
-      <c r="V3" s="5">
-        <v>7</v>
-      </c>
-      <c r="W3" s="5">
-        <v>7</v>
-      </c>
-      <c r="X3" s="5">
-        <v>7</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>7</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>7</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5">
-        <v>1</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1</v>
-      </c>
-      <c r="M4" s="5">
-        <v>1</v>
-      </c>
-      <c r="N4" s="5">
-        <v>1</v>
-      </c>
-      <c r="O4" s="5">
-        <v>1</v>
-      </c>
-      <c r="P4" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>1</v>
-      </c>
-      <c r="R4" s="5">
-        <v>0</v>
-      </c>
-      <c r="S4" s="5">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5">
-        <v>0</v>
-      </c>
-      <c r="V4" s="5">
-        <v>0</v>
-      </c>
-      <c r="W4" s="5">
-        <v>0</v>
-      </c>
-      <c r="X4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5">
-        <v>3</v>
-      </c>
-      <c r="G5" s="5">
-        <v>3</v>
-      </c>
-      <c r="H5" s="5">
-        <v>3</v>
-      </c>
-      <c r="I5" s="5">
-        <v>3</v>
-      </c>
-      <c r="J5" s="5">
-        <v>3</v>
-      </c>
-      <c r="K5" s="5">
-        <v>3</v>
-      </c>
-      <c r="L5" s="5">
-        <v>3</v>
-      </c>
-      <c r="M5" s="5">
-        <v>3</v>
-      </c>
-      <c r="N5" s="5">
-        <v>3</v>
-      </c>
-      <c r="O5" s="5">
-        <v>3</v>
-      </c>
-      <c r="P5" s="5">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>3</v>
-      </c>
-      <c r="R5" s="5">
-        <v>3</v>
-      </c>
-      <c r="S5" s="5">
-        <v>3</v>
-      </c>
-      <c r="T5" s="5">
-        <v>3</v>
-      </c>
-      <c r="U5" s="5">
-        <v>3</v>
-      </c>
-      <c r="V5" s="5">
-        <v>3</v>
-      </c>
-      <c r="W5" s="5">
-        <v>3</v>
-      </c>
-      <c r="X5" s="5">
-        <v>3</v>
-      </c>
-      <c r="Y5" s="5">
-        <v>3</v>
-      </c>
-      <c r="Z5" s="5">
-        <v>3</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5">
-        <v>10</v>
-      </c>
-      <c r="G6" s="5">
-        <v>10</v>
-      </c>
-      <c r="H6" s="5">
-        <v>10</v>
-      </c>
-      <c r="I6" s="5">
-        <v>10</v>
-      </c>
-      <c r="J6" s="5">
-        <v>10</v>
-      </c>
-      <c r="K6" s="5">
-        <v>10</v>
-      </c>
-      <c r="L6" s="5">
-        <v>10</v>
-      </c>
-      <c r="M6" s="5">
-        <v>10</v>
-      </c>
-      <c r="N6" s="5">
-        <v>10</v>
-      </c>
-      <c r="O6" s="5">
-        <v>10</v>
-      </c>
-      <c r="P6" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>10</v>
-      </c>
-      <c r="R6" s="5">
-        <v>10</v>
-      </c>
-      <c r="S6" s="5">
-        <v>10</v>
-      </c>
-      <c r="T6" s="5">
-        <v>10</v>
-      </c>
-      <c r="U6" s="5">
-        <v>10</v>
-      </c>
-      <c r="V6" s="5">
-        <v>10</v>
-      </c>
-      <c r="W6" s="5">
-        <v>10</v>
-      </c>
-      <c r="X6" s="5">
-        <v>10</v>
-      </c>
-      <c r="Y6" s="5">
-        <v>10</v>
-      </c>
-      <c r="Z6" s="5">
-        <v>10</v>
-      </c>
-      <c r="AA6" s="5">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4510,21 +4210,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B80F836-AAFA-4D20-813C-A31BE68F85E1}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.4140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -4535,16 +4236,22 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4554,17 +4261,23 @@
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2">
         <v>6000</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4574,17 +4287,23 @@
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>5000</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>2023</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -4594,17 +4313,23 @@
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>2000</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>2022</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4614,14 +4339,534 @@
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>2000</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>2019</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EB8FDB-F47B-40C2-8266-6700BCAB2D8C}">
+  <dimension ref="A1:AA6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1">
+        <v>2025</v>
+      </c>
+      <c r="C1">
+        <v>2026</v>
+      </c>
+      <c r="D1">
+        <v>2027</v>
+      </c>
+      <c r="E1">
+        <v>2028</v>
+      </c>
+      <c r="F1">
+        <v>2029</v>
+      </c>
+      <c r="G1">
+        <v>2030</v>
+      </c>
+      <c r="H1">
+        <v>2031</v>
+      </c>
+      <c r="I1">
+        <v>2032</v>
+      </c>
+      <c r="J1">
+        <v>2033</v>
+      </c>
+      <c r="K1">
+        <v>2034</v>
+      </c>
+      <c r="L1">
+        <v>2035</v>
+      </c>
+      <c r="M1">
+        <v>2036</v>
+      </c>
+      <c r="N1">
+        <v>2037</v>
+      </c>
+      <c r="O1">
+        <v>2038</v>
+      </c>
+      <c r="P1">
+        <v>2039</v>
+      </c>
+      <c r="Q1">
+        <v>2040</v>
+      </c>
+      <c r="R1">
+        <v>2041</v>
+      </c>
+      <c r="S1">
+        <v>2042</v>
+      </c>
+      <c r="T1">
+        <v>2043</v>
+      </c>
+      <c r="U1">
+        <v>2044</v>
+      </c>
+      <c r="V1">
+        <v>2045</v>
+      </c>
+      <c r="W1">
+        <v>2046</v>
+      </c>
+      <c r="X1">
+        <v>2047</v>
+      </c>
+      <c r="Y1">
+        <v>2048</v>
+      </c>
+      <c r="Z1">
+        <v>2049</v>
+      </c>
+      <c r="AA1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5">
+        <v>15</v>
+      </c>
+      <c r="K2" s="5">
+        <v>15</v>
+      </c>
+      <c r="L2" s="5">
+        <v>15</v>
+      </c>
+      <c r="M2" s="5">
+        <v>15</v>
+      </c>
+      <c r="N2" s="5">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5">
+        <v>15</v>
+      </c>
+      <c r="P2" s="5">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>15</v>
+      </c>
+      <c r="R2" s="5">
+        <v>15</v>
+      </c>
+      <c r="S2" s="5">
+        <v>15</v>
+      </c>
+      <c r="T2" s="5">
+        <v>15</v>
+      </c>
+      <c r="U2" s="5">
+        <v>15</v>
+      </c>
+      <c r="V2" s="5">
+        <v>15</v>
+      </c>
+      <c r="W2" s="5">
+        <v>15</v>
+      </c>
+      <c r="X2" s="5">
+        <v>15</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>15</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5">
+        <v>7</v>
+      </c>
+      <c r="H3" s="5">
+        <v>7</v>
+      </c>
+      <c r="I3" s="5">
+        <v>7</v>
+      </c>
+      <c r="J3" s="5">
+        <v>7</v>
+      </c>
+      <c r="K3" s="5">
+        <v>7</v>
+      </c>
+      <c r="L3" s="5">
+        <v>7</v>
+      </c>
+      <c r="M3" s="5">
+        <v>7</v>
+      </c>
+      <c r="N3" s="5">
+        <v>7</v>
+      </c>
+      <c r="O3" s="5">
+        <v>7</v>
+      </c>
+      <c r="P3" s="5">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>7</v>
+      </c>
+      <c r="R3" s="5">
+        <v>7</v>
+      </c>
+      <c r="S3" s="5">
+        <v>7</v>
+      </c>
+      <c r="T3" s="5">
+        <v>7</v>
+      </c>
+      <c r="U3" s="5">
+        <v>7</v>
+      </c>
+      <c r="V3" s="5">
+        <v>7</v>
+      </c>
+      <c r="W3" s="5">
+        <v>7</v>
+      </c>
+      <c r="X3" s="5">
+        <v>7</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0</v>
+      </c>
+      <c r="X4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="5">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5">
+        <v>3</v>
+      </c>
+      <c r="K5" s="5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="5">
+        <v>3</v>
+      </c>
+      <c r="N5" s="5">
+        <v>3</v>
+      </c>
+      <c r="O5" s="5">
+        <v>3</v>
+      </c>
+      <c r="P5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>3</v>
+      </c>
+      <c r="R5" s="5">
+        <v>3</v>
+      </c>
+      <c r="S5" s="5">
+        <v>3</v>
+      </c>
+      <c r="T5" s="5">
+        <v>3</v>
+      </c>
+      <c r="U5" s="5">
+        <v>3</v>
+      </c>
+      <c r="V5" s="5">
+        <v>3</v>
+      </c>
+      <c r="W5" s="5">
+        <v>3</v>
+      </c>
+      <c r="X5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>10</v>
+      </c>
+      <c r="G6" s="5">
+        <v>10</v>
+      </c>
+      <c r="H6" s="5">
+        <v>10</v>
+      </c>
+      <c r="I6" s="5">
+        <v>10</v>
+      </c>
+      <c r="J6" s="5">
+        <v>10</v>
+      </c>
+      <c r="K6" s="5">
+        <v>10</v>
+      </c>
+      <c r="L6" s="5">
+        <v>10</v>
+      </c>
+      <c r="M6" s="5">
+        <v>10</v>
+      </c>
+      <c r="N6" s="5">
+        <v>10</v>
+      </c>
+      <c r="O6" s="5">
+        <v>10</v>
+      </c>
+      <c r="P6" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>10</v>
+      </c>
+      <c r="R6" s="5">
+        <v>10</v>
+      </c>
+      <c r="S6" s="5">
+        <v>10</v>
+      </c>
+      <c r="T6" s="5">
+        <v>10</v>
+      </c>
+      <c r="U6" s="5">
+        <v>10</v>
+      </c>
+      <c r="V6" s="5">
+        <v>10</v>
+      </c>
+      <c r="W6" s="5">
+        <v>10</v>
+      </c>
+      <c r="X6" s="5">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4638,9 +4883,9 @@
       <selection activeCell="Q3" sqref="Q3:AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -4723,7 +4968,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4806,7 +5051,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -4889,7 +5134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -4972,7 +5217,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" ht="34" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -5095,9 +5340,9 @@
       <selection activeCell="B5" sqref="B5:AA5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -5180,7 +5425,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5289,7 +5534,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5398,7 +5643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -5507,7 +5752,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" ht="34" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -5630,9 +5875,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -5715,7 +5960,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5824,7 +6069,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5933,7 +6178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -6042,7 +6287,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" ht="34" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -6161,18 +6406,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5339A0-3D98-43CE-86F7-53EF60721306}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -6183,7 +6428,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6194,7 +6439,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6205,7 +6450,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -6216,7 +6461,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -6241,9 +6486,9 @@
       <selection sqref="A1:AA5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -6326,7 +6571,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6409,7 +6654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6492,7 +6737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -6575,7 +6820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" ht="34" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -6668,17 +6913,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E46CCB1-2754-42FA-B5C9-8DABA83A320C}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AA2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -6761,7 +7006,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -6854,13 +7099,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D074F1A1-9C61-4352-AF1E-453C90E48727}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -6943,7 +7188,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>53</v>
       </c>

</xml_diff>